<commit_message>
bao gia anh tuanbg
</commit_message>
<xml_diff>
--- a/5. WS/1. Bộ phận bảo hành/1. Thực hiện sửa chữa bảo hành/nam2022/Thang10/2.XulyBH/XLBH2210_AnhTuanBG.xlsx
+++ b/5. WS/1. Bộ phận bảo hành/1. Thực hiện sửa chữa bảo hành/nam2022/Thang10/2.XulyBH/XLBH2210_AnhTuanBG.xlsx
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="730" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="806" uniqueCount="125">
   <si>
     <t>STT</t>
   </si>
@@ -371,6 +371,60 @@
   <si>
     <t>125.212.203.114,16363</t>
   </si>
+  <si>
+    <t>Xử lý lại main, nâng cấp khay sim</t>
+  </si>
+  <si>
+    <t>Thay module GSM</t>
+  </si>
+  <si>
+    <t>Thiết bị reset liên tục</t>
+  </si>
+  <si>
+    <t>Nạp lại FW, nâng cấp khay sim</t>
+  </si>
+  <si>
+    <t>LK,NCFW</t>
+  </si>
+  <si>
+    <t>SE.4.00.---06.200630</t>
+  </si>
+  <si>
+    <t>Nạp lại FW</t>
+  </si>
+  <si>
+    <t>Thiết bị lỗi flash</t>
+  </si>
+  <si>
+    <t>Thay flash</t>
+  </si>
+  <si>
+    <t>SE.4.00.---05.190820</t>
+  </si>
+  <si>
+    <t>X.4.0.0.00002.180125</t>
+  </si>
+  <si>
+    <t>Cháy led GPS</t>
+  </si>
+  <si>
+    <t>Thay led GSP</t>
+  </si>
+  <si>
+    <t>B.2.27B</t>
+  </si>
+  <si>
+    <t>125.212.203.114,14848</t>
+  </si>
+  <si>
+    <t>Thiết bị treo</t>
+  </si>
+  <si>
+    <t>Cấu hình lại thiết bị</t>
+  </si>
+  <si>
+    <t>ID cũ: 000001504091105, hết hạn dịch vụ</t>
+  </si>
 </sst>
 </file>
 
@@ -597,7 +651,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="106">
+  <cellXfs count="107">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -864,28 +918,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="10" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -905,6 +938,30 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1251,40 +1308,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="99"/>
-      <c r="B1" s="99"/>
-      <c r="C1" s="99"/>
-      <c r="D1" s="99"/>
-      <c r="E1" s="99"/>
-      <c r="F1" s="99"/>
-      <c r="G1" s="99"/>
-      <c r="H1" s="99"/>
-      <c r="I1" s="99"/>
-      <c r="J1" s="99"/>
-      <c r="K1" s="99"/>
-      <c r="L1" s="99"/>
-      <c r="M1" s="99"/>
-      <c r="N1" s="99"/>
-      <c r="O1" s="99"/>
-      <c r="P1" s="99"/>
-      <c r="Q1" s="99"/>
-      <c r="R1" s="99"/>
-      <c r="S1" s="99"/>
-      <c r="T1" s="99"/>
-      <c r="U1" s="99"/>
-      <c r="V1" s="99"/>
+      <c r="A1" s="92"/>
+      <c r="B1" s="92"/>
+      <c r="C1" s="92"/>
+      <c r="D1" s="92"/>
+      <c r="E1" s="92"/>
+      <c r="F1" s="92"/>
+      <c r="G1" s="92"/>
+      <c r="H1" s="92"/>
+      <c r="I1" s="92"/>
+      <c r="J1" s="92"/>
+      <c r="K1" s="92"/>
+      <c r="L1" s="92"/>
+      <c r="M1" s="92"/>
+      <c r="N1" s="92"/>
+      <c r="O1" s="92"/>
+      <c r="P1" s="92"/>
+      <c r="Q1" s="92"/>
+      <c r="R1" s="92"/>
+      <c r="S1" s="92"/>
+      <c r="T1" s="92"/>
+      <c r="U1" s="92"/>
+      <c r="V1" s="92"/>
     </row>
     <row r="2" spans="1:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="100" t="s">
+      <c r="A2" s="93" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="101"/>
-      <c r="C2" s="101"/>
-      <c r="D2" s="101"/>
-      <c r="E2" s="102" t="s">
+      <c r="B2" s="94"/>
+      <c r="C2" s="94"/>
+      <c r="D2" s="94"/>
+      <c r="E2" s="95" t="s">
         <v>64</v>
       </c>
-      <c r="F2" s="102"/>
+      <c r="F2" s="95"/>
       <c r="G2" s="4"/>
       <c r="H2" s="20"/>
       <c r="I2" s="48"/>
@@ -1327,57 +1384,57 @@
       <c r="V3" s="27"/>
     </row>
     <row r="4" spans="1:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="103" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" s="98" t="s">
+      <c r="A4" s="96" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="91" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="98"/>
-      <c r="D4" s="98"/>
-      <c r="E4" s="98"/>
-      <c r="F4" s="98"/>
-      <c r="G4" s="98"/>
-      <c r="H4" s="98"/>
-      <c r="I4" s="98"/>
-      <c r="J4" s="98" t="s">
+      <c r="C4" s="91"/>
+      <c r="D4" s="91"/>
+      <c r="E4" s="91"/>
+      <c r="F4" s="91"/>
+      <c r="G4" s="91"/>
+      <c r="H4" s="91"/>
+      <c r="I4" s="91"/>
+      <c r="J4" s="91" t="s">
         <v>6</v>
       </c>
-      <c r="K4" s="98" t="s">
+      <c r="K4" s="91" t="s">
         <v>11</v>
       </c>
-      <c r="L4" s="98"/>
-      <c r="M4" s="95" t="s">
+      <c r="L4" s="91"/>
+      <c r="M4" s="97" t="s">
         <v>42</v>
       </c>
-      <c r="N4" s="95" t="s">
+      <c r="N4" s="97" t="s">
         <v>10</v>
       </c>
-      <c r="O4" s="95" t="s">
+      <c r="O4" s="97" t="s">
         <v>7</v>
       </c>
-      <c r="P4" s="93" t="s">
+      <c r="P4" s="102" t="s">
         <v>14</v>
       </c>
-      <c r="Q4" s="95" t="s">
+      <c r="Q4" s="97" t="s">
         <v>39</v>
       </c>
-      <c r="R4" s="95" t="s">
+      <c r="R4" s="97" t="s">
         <v>53</v>
       </c>
-      <c r="S4" s="97" t="s">
+      <c r="S4" s="104" t="s">
         <v>54</v>
       </c>
       <c r="T4" s="26"/>
-      <c r="U4" s="98" t="s">
+      <c r="U4" s="91" t="s">
         <v>39</v>
       </c>
-      <c r="V4" s="98" t="s">
+      <c r="V4" s="91" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="5" spans="1:22" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="103"/>
+      <c r="A5" s="96"/>
       <c r="B5" s="66" t="s">
         <v>1</v>
       </c>
@@ -1402,23 +1459,23 @@
       <c r="I5" s="50" t="s">
         <v>15</v>
       </c>
-      <c r="J5" s="98"/>
+      <c r="J5" s="91"/>
       <c r="K5" s="66" t="s">
         <v>12</v>
       </c>
       <c r="L5" s="66" t="s">
         <v>13</v>
       </c>
-      <c r="M5" s="96"/>
-      <c r="N5" s="96"/>
-      <c r="O5" s="96"/>
-      <c r="P5" s="94"/>
-      <c r="Q5" s="96"/>
-      <c r="R5" s="96"/>
-      <c r="S5" s="97"/>
+      <c r="M5" s="98"/>
+      <c r="N5" s="98"/>
+      <c r="O5" s="98"/>
+      <c r="P5" s="103"/>
+      <c r="Q5" s="98"/>
+      <c r="R5" s="98"/>
+      <c r="S5" s="104"/>
       <c r="T5" s="26"/>
-      <c r="U5" s="98"/>
-      <c r="V5" s="98"/>
+      <c r="U5" s="91"/>
+      <c r="V5" s="91"/>
     </row>
     <row r="6" spans="1:22" s="11" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
@@ -1451,7 +1508,7 @@
       <c r="R6" s="83"/>
       <c r="S6" s="84"/>
       <c r="T6" s="67"/>
-      <c r="U6" s="90" t="s">
+      <c r="U6" s="99" t="s">
         <v>18</v>
       </c>
       <c r="V6" s="3" t="s">
@@ -1509,7 +1566,7 @@
       </c>
       <c r="S7" s="84"/>
       <c r="T7" s="67"/>
-      <c r="U7" s="91"/>
+      <c r="U7" s="100"/>
       <c r="V7" s="3" t="s">
         <v>35</v>
       </c>
@@ -1537,7 +1594,7 @@
       <c r="R8" s="83"/>
       <c r="S8" s="84"/>
       <c r="T8" s="67"/>
-      <c r="U8" s="91"/>
+      <c r="U8" s="100"/>
       <c r="V8" s="3" t="s">
         <v>21</v>
       </c>
@@ -1565,7 +1622,7 @@
       <c r="R9" s="83"/>
       <c r="S9" s="84"/>
       <c r="T9" s="67"/>
-      <c r="U9" s="91"/>
+      <c r="U9" s="100"/>
       <c r="V9" s="3" t="s">
         <v>51</v>
       </c>
@@ -1593,7 +1650,7 @@
       <c r="R10" s="83"/>
       <c r="S10" s="84"/>
       <c r="T10" s="67"/>
-      <c r="U10" s="91"/>
+      <c r="U10" s="100"/>
       <c r="V10" s="3" t="s">
         <v>31</v>
       </c>
@@ -1621,7 +1678,7 @@
       <c r="R11" s="83"/>
       <c r="S11" s="84"/>
       <c r="T11" s="67"/>
-      <c r="U11" s="91"/>
+      <c r="U11" s="100"/>
       <c r="V11" s="3" t="s">
         <v>30</v>
       </c>
@@ -1649,7 +1706,7 @@
       <c r="R12" s="83"/>
       <c r="S12" s="84"/>
       <c r="T12" s="67"/>
-      <c r="U12" s="90" t="s">
+      <c r="U12" s="99" t="s">
         <v>19</v>
       </c>
       <c r="V12" s="3" t="s">
@@ -1679,7 +1736,7 @@
       <c r="R13" s="83"/>
       <c r="S13" s="84"/>
       <c r="T13" s="67"/>
-      <c r="U13" s="91"/>
+      <c r="U13" s="100"/>
       <c r="V13" s="3" t="s">
         <v>37</v>
       </c>
@@ -1707,7 +1764,7 @@
       <c r="R14" s="83"/>
       <c r="S14" s="84"/>
       <c r="T14" s="67"/>
-      <c r="U14" s="91"/>
+      <c r="U14" s="100"/>
       <c r="V14" s="3" t="s">
         <v>36</v>
       </c>
@@ -1735,7 +1792,7 @@
       <c r="R15" s="83"/>
       <c r="S15" s="84"/>
       <c r="T15" s="13"/>
-      <c r="U15" s="91"/>
+      <c r="U15" s="100"/>
       <c r="V15" s="3" t="s">
         <v>24</v>
       </c>
@@ -1763,7 +1820,7 @@
       <c r="R16" s="83"/>
       <c r="S16" s="84"/>
       <c r="T16" s="13"/>
-      <c r="U16" s="92"/>
+      <c r="U16" s="101"/>
       <c r="V16" s="3" t="s">
         <v>25</v>
       </c>
@@ -3173,6 +3230,13 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="U6:U11"/>
+    <mergeCell ref="U12:U16"/>
+    <mergeCell ref="P4:P5"/>
+    <mergeCell ref="Q4:Q5"/>
+    <mergeCell ref="R4:R5"/>
+    <mergeCell ref="S4:S5"/>
+    <mergeCell ref="U4:U5"/>
     <mergeCell ref="V4:V5"/>
     <mergeCell ref="A1:V1"/>
     <mergeCell ref="A2:D2"/>
@@ -3184,13 +3248,6 @@
     <mergeCell ref="M4:M5"/>
     <mergeCell ref="N4:N5"/>
     <mergeCell ref="O4:O5"/>
-    <mergeCell ref="U6:U11"/>
-    <mergeCell ref="U12:U16"/>
-    <mergeCell ref="P4:P5"/>
-    <mergeCell ref="Q4:Q5"/>
-    <mergeCell ref="R4:R5"/>
-    <mergeCell ref="S4:S5"/>
-    <mergeCell ref="U4:U5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3234,41 +3291,41 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="99"/>
-      <c r="B1" s="99"/>
-      <c r="C1" s="99"/>
-      <c r="D1" s="99"/>
-      <c r="E1" s="99"/>
-      <c r="F1" s="99"/>
-      <c r="G1" s="99"/>
-      <c r="H1" s="99"/>
-      <c r="I1" s="99"/>
-      <c r="J1" s="99"/>
-      <c r="K1" s="99"/>
-      <c r="L1" s="99"/>
-      <c r="M1" s="99"/>
-      <c r="N1" s="99"/>
-      <c r="O1" s="99"/>
-      <c r="P1" s="99"/>
-      <c r="Q1" s="99"/>
-      <c r="R1" s="99"/>
-      <c r="S1" s="99"/>
-      <c r="T1" s="99"/>
-      <c r="U1" s="99"/>
-      <c r="V1" s="99"/>
+      <c r="A1" s="92"/>
+      <c r="B1" s="92"/>
+      <c r="C1" s="92"/>
+      <c r="D1" s="92"/>
+      <c r="E1" s="92"/>
+      <c r="F1" s="92"/>
+      <c r="G1" s="92"/>
+      <c r="H1" s="92"/>
+      <c r="I1" s="92"/>
+      <c r="J1" s="92"/>
+      <c r="K1" s="92"/>
+      <c r="L1" s="92"/>
+      <c r="M1" s="92"/>
+      <c r="N1" s="92"/>
+      <c r="O1" s="92"/>
+      <c r="P1" s="92"/>
+      <c r="Q1" s="92"/>
+      <c r="R1" s="92"/>
+      <c r="S1" s="92"/>
+      <c r="T1" s="92"/>
+      <c r="U1" s="92"/>
+      <c r="V1" s="92"/>
       <c r="W1" s="44"/>
     </row>
     <row r="2" spans="1:23" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="100" t="s">
+      <c r="A2" s="93" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="101"/>
-      <c r="C2" s="101"/>
-      <c r="D2" s="101"/>
-      <c r="E2" s="104" t="s">
+      <c r="B2" s="94"/>
+      <c r="C2" s="94"/>
+      <c r="D2" s="94"/>
+      <c r="E2" s="105" t="s">
         <v>64</v>
       </c>
-      <c r="F2" s="104"/>
+      <c r="F2" s="105"/>
       <c r="G2" s="4"/>
       <c r="H2" s="20"/>
       <c r="I2" s="48"/>
@@ -3313,58 +3370,58 @@
       <c r="W3" s="26"/>
     </row>
     <row r="4" spans="1:23" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="103" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" s="98" t="s">
+      <c r="A4" s="96" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="91" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="98"/>
-      <c r="D4" s="98"/>
-      <c r="E4" s="98"/>
-      <c r="F4" s="98"/>
-      <c r="G4" s="98"/>
-      <c r="H4" s="98"/>
-      <c r="I4" s="98"/>
-      <c r="J4" s="98" t="s">
+      <c r="C4" s="91"/>
+      <c r="D4" s="91"/>
+      <c r="E4" s="91"/>
+      <c r="F4" s="91"/>
+      <c r="G4" s="91"/>
+      <c r="H4" s="91"/>
+      <c r="I4" s="91"/>
+      <c r="J4" s="91" t="s">
         <v>6</v>
       </c>
-      <c r="K4" s="98" t="s">
+      <c r="K4" s="91" t="s">
         <v>11</v>
       </c>
-      <c r="L4" s="98"/>
-      <c r="M4" s="95" t="s">
+      <c r="L4" s="91"/>
+      <c r="M4" s="97" t="s">
         <v>42</v>
       </c>
-      <c r="N4" s="95" t="s">
+      <c r="N4" s="97" t="s">
         <v>10</v>
       </c>
-      <c r="O4" s="95" t="s">
+      <c r="O4" s="97" t="s">
         <v>7</v>
       </c>
-      <c r="P4" s="93" t="s">
+      <c r="P4" s="102" t="s">
         <v>14</v>
       </c>
-      <c r="Q4" s="95" t="s">
+      <c r="Q4" s="97" t="s">
         <v>39</v>
       </c>
-      <c r="R4" s="95" t="s">
+      <c r="R4" s="97" t="s">
         <v>53</v>
       </c>
-      <c r="S4" s="97" t="s">
+      <c r="S4" s="104" t="s">
         <v>54</v>
       </c>
       <c r="T4" s="26"/>
-      <c r="U4" s="98" t="s">
+      <c r="U4" s="91" t="s">
         <v>39</v>
       </c>
-      <c r="V4" s="98" t="s">
+      <c r="V4" s="91" t="s">
         <v>53</v>
       </c>
       <c r="W4" s="45"/>
     </row>
     <row r="5" spans="1:23" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="103"/>
+      <c r="A5" s="96"/>
       <c r="B5" s="66" t="s">
         <v>1</v>
       </c>
@@ -3389,23 +3446,23 @@
       <c r="I5" s="50" t="s">
         <v>15</v>
       </c>
-      <c r="J5" s="98"/>
+      <c r="J5" s="91"/>
       <c r="K5" s="66" t="s">
         <v>12</v>
       </c>
       <c r="L5" s="66" t="s">
         <v>13</v>
       </c>
-      <c r="M5" s="96"/>
-      <c r="N5" s="96"/>
-      <c r="O5" s="96"/>
-      <c r="P5" s="94"/>
-      <c r="Q5" s="96"/>
-      <c r="R5" s="96"/>
-      <c r="S5" s="97"/>
+      <c r="M5" s="98"/>
+      <c r="N5" s="98"/>
+      <c r="O5" s="98"/>
+      <c r="P5" s="103"/>
+      <c r="Q5" s="98"/>
+      <c r="R5" s="98"/>
+      <c r="S5" s="104"/>
       <c r="T5" s="26"/>
-      <c r="U5" s="98"/>
-      <c r="V5" s="98"/>
+      <c r="U5" s="91"/>
+      <c r="V5" s="91"/>
       <c r="W5" s="45"/>
     </row>
     <row r="6" spans="1:23" s="11" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -3455,7 +3512,7 @@
       </c>
       <c r="S6" s="84"/>
       <c r="T6" s="67"/>
-      <c r="U6" s="90" t="s">
+      <c r="U6" s="99" t="s">
         <v>18</v>
       </c>
       <c r="V6" s="3" t="s">
@@ -3510,7 +3567,7 @@
       </c>
       <c r="S7" s="84"/>
       <c r="T7" s="67"/>
-      <c r="U7" s="91"/>
+      <c r="U7" s="100"/>
       <c r="V7" s="3" t="s">
         <v>35</v>
       </c>
@@ -3539,7 +3596,7 @@
       <c r="R8" s="83"/>
       <c r="S8" s="84"/>
       <c r="T8" s="67"/>
-      <c r="U8" s="91"/>
+      <c r="U8" s="100"/>
       <c r="V8" s="3" t="s">
         <v>21</v>
       </c>
@@ -3568,7 +3625,7 @@
       <c r="R9" s="83"/>
       <c r="S9" s="84"/>
       <c r="T9" s="67"/>
-      <c r="U9" s="91"/>
+      <c r="U9" s="100"/>
       <c r="V9" s="3" t="s">
         <v>51</v>
       </c>
@@ -3597,7 +3654,7 @@
       <c r="R10" s="83"/>
       <c r="S10" s="84"/>
       <c r="T10" s="67"/>
-      <c r="U10" s="91"/>
+      <c r="U10" s="100"/>
       <c r="V10" s="3" t="s">
         <v>31</v>
       </c>
@@ -3626,7 +3683,7 @@
       <c r="R11" s="83"/>
       <c r="S11" s="84"/>
       <c r="T11" s="67"/>
-      <c r="U11" s="91"/>
+      <c r="U11" s="100"/>
       <c r="V11" s="3" t="s">
         <v>30</v>
       </c>
@@ -3655,7 +3712,7 @@
       <c r="R12" s="83"/>
       <c r="S12" s="84"/>
       <c r="T12" s="67"/>
-      <c r="U12" s="90" t="s">
+      <c r="U12" s="99" t="s">
         <v>19</v>
       </c>
       <c r="V12" s="3" t="s">
@@ -3686,7 +3743,7 @@
       <c r="R13" s="83"/>
       <c r="S13" s="84"/>
       <c r="T13" s="67"/>
-      <c r="U13" s="91"/>
+      <c r="U13" s="100"/>
       <c r="V13" s="3" t="s">
         <v>37</v>
       </c>
@@ -3715,7 +3772,7 @@
       <c r="R14" s="83"/>
       <c r="S14" s="84"/>
       <c r="T14" s="67"/>
-      <c r="U14" s="91"/>
+      <c r="U14" s="100"/>
       <c r="V14" s="3" t="s">
         <v>36</v>
       </c>
@@ -3744,7 +3801,7 @@
       <c r="R15" s="83"/>
       <c r="S15" s="84"/>
       <c r="T15" s="13"/>
-      <c r="U15" s="91"/>
+      <c r="U15" s="100"/>
       <c r="V15" s="3" t="s">
         <v>24</v>
       </c>
@@ -3773,7 +3830,7 @@
       <c r="R16" s="83"/>
       <c r="S16" s="84"/>
       <c r="T16" s="13"/>
-      <c r="U16" s="92"/>
+      <c r="U16" s="101"/>
       <c r="V16" s="3" t="s">
         <v>25</v>
       </c>
@@ -5241,6 +5298,13 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="U6:U11"/>
+    <mergeCell ref="U12:U16"/>
+    <mergeCell ref="P4:P5"/>
+    <mergeCell ref="Q4:Q5"/>
+    <mergeCell ref="R4:R5"/>
+    <mergeCell ref="S4:S5"/>
+    <mergeCell ref="U4:U5"/>
     <mergeCell ref="V4:V5"/>
     <mergeCell ref="A1:V1"/>
     <mergeCell ref="A2:D2"/>
@@ -5252,13 +5316,6 @@
     <mergeCell ref="M4:M5"/>
     <mergeCell ref="N4:N5"/>
     <mergeCell ref="O4:O5"/>
-    <mergeCell ref="U6:U11"/>
-    <mergeCell ref="U12:U16"/>
-    <mergeCell ref="P4:P5"/>
-    <mergeCell ref="Q4:Q5"/>
-    <mergeCell ref="R4:R5"/>
-    <mergeCell ref="S4:S5"/>
-    <mergeCell ref="U4:U5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -5302,41 +5359,41 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="99"/>
-      <c r="B1" s="99"/>
-      <c r="C1" s="99"/>
-      <c r="D1" s="99"/>
-      <c r="E1" s="99"/>
-      <c r="F1" s="99"/>
-      <c r="G1" s="99"/>
-      <c r="H1" s="99"/>
-      <c r="I1" s="99"/>
-      <c r="J1" s="99"/>
-      <c r="K1" s="99"/>
-      <c r="L1" s="99"/>
-      <c r="M1" s="99"/>
-      <c r="N1" s="99"/>
-      <c r="O1" s="99"/>
-      <c r="P1" s="99"/>
-      <c r="Q1" s="99"/>
-      <c r="R1" s="99"/>
-      <c r="S1" s="99"/>
-      <c r="T1" s="99"/>
-      <c r="U1" s="99"/>
-      <c r="V1" s="99"/>
+      <c r="A1" s="92"/>
+      <c r="B1" s="92"/>
+      <c r="C1" s="92"/>
+      <c r="D1" s="92"/>
+      <c r="E1" s="92"/>
+      <c r="F1" s="92"/>
+      <c r="G1" s="92"/>
+      <c r="H1" s="92"/>
+      <c r="I1" s="92"/>
+      <c r="J1" s="92"/>
+      <c r="K1" s="92"/>
+      <c r="L1" s="92"/>
+      <c r="M1" s="92"/>
+      <c r="N1" s="92"/>
+      <c r="O1" s="92"/>
+      <c r="P1" s="92"/>
+      <c r="Q1" s="92"/>
+      <c r="R1" s="92"/>
+      <c r="S1" s="92"/>
+      <c r="T1" s="92"/>
+      <c r="U1" s="92"/>
+      <c r="V1" s="92"/>
       <c r="W1" s="44"/>
     </row>
     <row r="2" spans="1:23" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="100" t="s">
+      <c r="A2" s="93" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="101"/>
-      <c r="C2" s="101"/>
-      <c r="D2" s="101"/>
-      <c r="E2" s="104" t="s">
+      <c r="B2" s="94"/>
+      <c r="C2" s="94"/>
+      <c r="D2" s="94"/>
+      <c r="E2" s="105" t="s">
         <v>64</v>
       </c>
-      <c r="F2" s="104"/>
+      <c r="F2" s="105"/>
       <c r="G2" s="4"/>
       <c r="H2" s="20"/>
       <c r="I2" s="48"/>
@@ -5381,58 +5438,58 @@
       <c r="W3" s="26"/>
     </row>
     <row r="4" spans="1:23" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="103" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" s="98" t="s">
+      <c r="A4" s="96" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="91" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="98"/>
-      <c r="D4" s="98"/>
-      <c r="E4" s="98"/>
-      <c r="F4" s="98"/>
-      <c r="G4" s="98"/>
-      <c r="H4" s="98"/>
-      <c r="I4" s="98"/>
-      <c r="J4" s="98" t="s">
+      <c r="C4" s="91"/>
+      <c r="D4" s="91"/>
+      <c r="E4" s="91"/>
+      <c r="F4" s="91"/>
+      <c r="G4" s="91"/>
+      <c r="H4" s="91"/>
+      <c r="I4" s="91"/>
+      <c r="J4" s="91" t="s">
         <v>6</v>
       </c>
-      <c r="K4" s="98" t="s">
+      <c r="K4" s="91" t="s">
         <v>11</v>
       </c>
-      <c r="L4" s="98"/>
-      <c r="M4" s="95" t="s">
+      <c r="L4" s="91"/>
+      <c r="M4" s="97" t="s">
         <v>42</v>
       </c>
-      <c r="N4" s="95" t="s">
+      <c r="N4" s="97" t="s">
         <v>10</v>
       </c>
-      <c r="O4" s="95" t="s">
+      <c r="O4" s="97" t="s">
         <v>7</v>
       </c>
-      <c r="P4" s="93" t="s">
+      <c r="P4" s="102" t="s">
         <v>14</v>
       </c>
-      <c r="Q4" s="95" t="s">
+      <c r="Q4" s="97" t="s">
         <v>39</v>
       </c>
-      <c r="R4" s="95" t="s">
+      <c r="R4" s="97" t="s">
         <v>53</v>
       </c>
-      <c r="S4" s="97" t="s">
+      <c r="S4" s="104" t="s">
         <v>54</v>
       </c>
       <c r="T4" s="26"/>
-      <c r="U4" s="98" t="s">
+      <c r="U4" s="91" t="s">
         <v>39</v>
       </c>
-      <c r="V4" s="98" t="s">
+      <c r="V4" s="91" t="s">
         <v>53</v>
       </c>
       <c r="W4" s="45"/>
     </row>
     <row r="5" spans="1:23" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="103"/>
+      <c r="A5" s="96"/>
       <c r="B5" s="66" t="s">
         <v>1</v>
       </c>
@@ -5457,23 +5514,23 @@
       <c r="I5" s="50" t="s">
         <v>15</v>
       </c>
-      <c r="J5" s="98"/>
+      <c r="J5" s="91"/>
       <c r="K5" s="66" t="s">
         <v>12</v>
       </c>
       <c r="L5" s="66" t="s">
         <v>13</v>
       </c>
-      <c r="M5" s="96"/>
-      <c r="N5" s="96"/>
-      <c r="O5" s="96"/>
-      <c r="P5" s="94"/>
-      <c r="Q5" s="96"/>
-      <c r="R5" s="96"/>
-      <c r="S5" s="97"/>
+      <c r="M5" s="98"/>
+      <c r="N5" s="98"/>
+      <c r="O5" s="98"/>
+      <c r="P5" s="103"/>
+      <c r="Q5" s="98"/>
+      <c r="R5" s="98"/>
+      <c r="S5" s="104"/>
       <c r="T5" s="26"/>
-      <c r="U5" s="98"/>
-      <c r="V5" s="98"/>
+      <c r="U5" s="91"/>
+      <c r="V5" s="91"/>
       <c r="W5" s="45"/>
     </row>
     <row r="6" spans="1:23" s="11" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -5525,7 +5582,7 @@
       </c>
       <c r="S6" s="74"/>
       <c r="T6" s="67"/>
-      <c r="U6" s="90" t="s">
+      <c r="U6" s="99" t="s">
         <v>18</v>
       </c>
       <c r="V6" s="3" t="s">
@@ -5580,7 +5637,7 @@
       </c>
       <c r="S7" s="74"/>
       <c r="T7" s="67"/>
-      <c r="U7" s="91"/>
+      <c r="U7" s="100"/>
       <c r="V7" s="3" t="s">
         <v>35</v>
       </c>
@@ -5637,7 +5694,7 @@
       </c>
       <c r="S8" s="74"/>
       <c r="T8" s="67"/>
-      <c r="U8" s="91"/>
+      <c r="U8" s="100"/>
       <c r="V8" s="3" t="s">
         <v>21</v>
       </c>
@@ -5692,7 +5749,7 @@
       </c>
       <c r="S9" s="74"/>
       <c r="T9" s="67"/>
-      <c r="U9" s="91"/>
+      <c r="U9" s="100"/>
       <c r="V9" s="3" t="s">
         <v>51</v>
       </c>
@@ -5749,7 +5806,7 @@
       </c>
       <c r="S10" s="74"/>
       <c r="T10" s="67"/>
-      <c r="U10" s="91"/>
+      <c r="U10" s="100"/>
       <c r="V10" s="3" t="s">
         <v>31</v>
       </c>
@@ -5778,7 +5835,7 @@
       <c r="R11" s="65"/>
       <c r="S11" s="74"/>
       <c r="T11" s="67"/>
-      <c r="U11" s="91"/>
+      <c r="U11" s="100"/>
       <c r="V11" s="3" t="s">
         <v>30</v>
       </c>
@@ -5807,7 +5864,7 @@
       <c r="R12" s="2"/>
       <c r="S12" s="3"/>
       <c r="T12" s="67"/>
-      <c r="U12" s="90" t="s">
+      <c r="U12" s="99" t="s">
         <v>19</v>
       </c>
       <c r="V12" s="3" t="s">
@@ -5838,7 +5895,7 @@
       <c r="R13" s="2"/>
       <c r="S13" s="3"/>
       <c r="T13" s="67"/>
-      <c r="U13" s="91"/>
+      <c r="U13" s="100"/>
       <c r="V13" s="3" t="s">
         <v>37</v>
       </c>
@@ -5867,7 +5924,7 @@
       <c r="R14" s="2"/>
       <c r="S14" s="3"/>
       <c r="T14" s="67"/>
-      <c r="U14" s="91"/>
+      <c r="U14" s="100"/>
       <c r="V14" s="3" t="s">
         <v>36</v>
       </c>
@@ -5896,7 +5953,7 @@
       <c r="R15" s="2"/>
       <c r="S15" s="3"/>
       <c r="T15" s="13"/>
-      <c r="U15" s="91"/>
+      <c r="U15" s="100"/>
       <c r="V15" s="3" t="s">
         <v>24</v>
       </c>
@@ -5925,7 +5982,7 @@
       <c r="R16" s="2"/>
       <c r="S16" s="3"/>
       <c r="T16" s="13"/>
-      <c r="U16" s="92"/>
+      <c r="U16" s="101"/>
       <c r="V16" s="3" t="s">
         <v>25</v>
       </c>
@@ -7631,6 +7688,13 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="U6:U11"/>
+    <mergeCell ref="U12:U16"/>
+    <mergeCell ref="P4:P5"/>
+    <mergeCell ref="Q4:Q5"/>
+    <mergeCell ref="R4:R5"/>
+    <mergeCell ref="S4:S5"/>
+    <mergeCell ref="U4:U5"/>
     <mergeCell ref="V4:V5"/>
     <mergeCell ref="A1:V1"/>
     <mergeCell ref="A2:D2"/>
@@ -7642,13 +7706,6 @@
     <mergeCell ref="M4:M5"/>
     <mergeCell ref="N4:N5"/>
     <mergeCell ref="O4:O5"/>
-    <mergeCell ref="U6:U11"/>
-    <mergeCell ref="U12:U16"/>
-    <mergeCell ref="P4:P5"/>
-    <mergeCell ref="Q4:Q5"/>
-    <mergeCell ref="R4:R5"/>
-    <mergeCell ref="S4:S5"/>
-    <mergeCell ref="U4:U5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -7659,8 +7716,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X115"/>
   <sheetViews>
-    <sheetView showZeros="0" tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView showZeros="0" tabSelected="1" topLeftCell="B1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -7692,41 +7749,41 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="99"/>
-      <c r="B1" s="99"/>
-      <c r="C1" s="99"/>
-      <c r="D1" s="99"/>
-      <c r="E1" s="99"/>
-      <c r="F1" s="99"/>
-      <c r="G1" s="99"/>
-      <c r="H1" s="99"/>
-      <c r="I1" s="99"/>
-      <c r="J1" s="99"/>
-      <c r="K1" s="99"/>
-      <c r="L1" s="99"/>
-      <c r="M1" s="99"/>
-      <c r="N1" s="99"/>
-      <c r="O1" s="99"/>
-      <c r="P1" s="99"/>
-      <c r="Q1" s="99"/>
-      <c r="R1" s="99"/>
-      <c r="S1" s="99"/>
-      <c r="T1" s="99"/>
-      <c r="U1" s="99"/>
-      <c r="V1" s="99"/>
+      <c r="A1" s="92"/>
+      <c r="B1" s="92"/>
+      <c r="C1" s="92"/>
+      <c r="D1" s="92"/>
+      <c r="E1" s="92"/>
+      <c r="F1" s="92"/>
+      <c r="G1" s="92"/>
+      <c r="H1" s="92"/>
+      <c r="I1" s="92"/>
+      <c r="J1" s="92"/>
+      <c r="K1" s="92"/>
+      <c r="L1" s="92"/>
+      <c r="M1" s="92"/>
+      <c r="N1" s="92"/>
+      <c r="O1" s="92"/>
+      <c r="P1" s="92"/>
+      <c r="Q1" s="92"/>
+      <c r="R1" s="92"/>
+      <c r="S1" s="92"/>
+      <c r="T1" s="92"/>
+      <c r="U1" s="92"/>
+      <c r="V1" s="92"/>
       <c r="W1" s="44"/>
     </row>
     <row r="2" spans="1:23" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="100" t="s">
+      <c r="A2" s="93" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="101"/>
-      <c r="C2" s="101"/>
-      <c r="D2" s="101"/>
-      <c r="E2" s="104" t="s">
+      <c r="B2" s="94"/>
+      <c r="C2" s="94"/>
+      <c r="D2" s="94"/>
+      <c r="E2" s="105" t="s">
         <v>64</v>
       </c>
-      <c r="F2" s="104"/>
+      <c r="F2" s="105"/>
       <c r="G2" s="4"/>
       <c r="H2" s="20"/>
       <c r="I2" s="48"/>
@@ -7771,58 +7828,58 @@
       <c r="W3" s="26"/>
     </row>
     <row r="4" spans="1:23" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="103" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" s="98" t="s">
+      <c r="A4" s="96" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="91" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="98"/>
-      <c r="D4" s="98"/>
-      <c r="E4" s="98"/>
-      <c r="F4" s="98"/>
-      <c r="G4" s="98"/>
-      <c r="H4" s="98"/>
-      <c r="I4" s="98"/>
-      <c r="J4" s="98" t="s">
+      <c r="C4" s="91"/>
+      <c r="D4" s="91"/>
+      <c r="E4" s="91"/>
+      <c r="F4" s="91"/>
+      <c r="G4" s="91"/>
+      <c r="H4" s="91"/>
+      <c r="I4" s="91"/>
+      <c r="J4" s="91" t="s">
         <v>6</v>
       </c>
-      <c r="K4" s="98" t="s">
+      <c r="K4" s="91" t="s">
         <v>11</v>
       </c>
-      <c r="L4" s="98"/>
-      <c r="M4" s="95" t="s">
+      <c r="L4" s="91"/>
+      <c r="M4" s="97" t="s">
         <v>42</v>
       </c>
-      <c r="N4" s="95" t="s">
+      <c r="N4" s="97" t="s">
         <v>10</v>
       </c>
-      <c r="O4" s="95" t="s">
+      <c r="O4" s="97" t="s">
         <v>7</v>
       </c>
-      <c r="P4" s="93" t="s">
+      <c r="P4" s="102" t="s">
         <v>14</v>
       </c>
-      <c r="Q4" s="95" t="s">
+      <c r="Q4" s="97" t="s">
         <v>39</v>
       </c>
-      <c r="R4" s="95" t="s">
+      <c r="R4" s="97" t="s">
         <v>53</v>
       </c>
-      <c r="S4" s="97" t="s">
+      <c r="S4" s="104" t="s">
         <v>54</v>
       </c>
       <c r="T4" s="26"/>
-      <c r="U4" s="98" t="s">
+      <c r="U4" s="91" t="s">
         <v>39</v>
       </c>
-      <c r="V4" s="98" t="s">
+      <c r="V4" s="91" t="s">
         <v>53</v>
       </c>
       <c r="W4" s="45"/>
     </row>
     <row r="5" spans="1:23" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="103"/>
+      <c r="A5" s="96"/>
       <c r="B5" s="66" t="s">
         <v>1</v>
       </c>
@@ -7847,57 +7904,73 @@
       <c r="I5" s="50" t="s">
         <v>15</v>
       </c>
-      <c r="J5" s="98"/>
+      <c r="J5" s="91"/>
       <c r="K5" s="66" t="s">
         <v>12</v>
       </c>
       <c r="L5" s="66" t="s">
         <v>13</v>
       </c>
-      <c r="M5" s="96"/>
-      <c r="N5" s="96"/>
-      <c r="O5" s="96"/>
-      <c r="P5" s="94"/>
-      <c r="Q5" s="96"/>
-      <c r="R5" s="96"/>
-      <c r="S5" s="97"/>
+      <c r="M5" s="98"/>
+      <c r="N5" s="98"/>
+      <c r="O5" s="98"/>
+      <c r="P5" s="103"/>
+      <c r="Q5" s="98"/>
+      <c r="R5" s="98"/>
+      <c r="S5" s="104"/>
       <c r="T5" s="26"/>
-      <c r="U5" s="98"/>
-      <c r="V5" s="98"/>
+      <c r="U5" s="91"/>
+      <c r="V5" s="91"/>
       <c r="W5" s="45"/>
     </row>
     <row r="6" spans="1:23" s="11" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="3">
+      <c r="A6" s="74">
         <v>1</v>
       </c>
       <c r="B6" s="59">
         <v>44861</v>
       </c>
       <c r="C6" s="59"/>
-      <c r="D6" s="57" t="s">
+      <c r="D6" s="60" t="s">
         <v>68</v>
       </c>
-      <c r="E6" s="58">
+      <c r="E6" s="73">
         <v>864811037169815</v>
       </c>
-      <c r="F6" s="57"/>
-      <c r="G6" s="57" t="s">
+      <c r="F6" s="60"/>
+      <c r="G6" s="60" t="s">
         <v>63</v>
       </c>
       <c r="H6" s="60"/>
-      <c r="I6" s="51"/>
-      <c r="J6" s="62"/>
+      <c r="I6" s="60" t="s">
+        <v>87</v>
+      </c>
+      <c r="J6" s="62" t="s">
+        <v>98</v>
+      </c>
       <c r="K6" s="63"/>
-      <c r="L6" s="1"/>
-      <c r="M6" s="64"/>
+      <c r="L6" s="73" t="s">
+        <v>103</v>
+      </c>
+      <c r="M6" s="64" t="s">
+        <v>107</v>
+      </c>
       <c r="N6" s="62"/>
-      <c r="O6" s="62"/>
-      <c r="P6" s="64"/>
-      <c r="Q6" s="62"/>
-      <c r="R6" s="65"/>
-      <c r="S6" s="3"/>
+      <c r="O6" s="62" t="s">
+        <v>77</v>
+      </c>
+      <c r="P6" s="64" t="s">
+        <v>78</v>
+      </c>
+      <c r="Q6" s="62" t="s">
+        <v>100</v>
+      </c>
+      <c r="R6" s="65" t="s">
+        <v>101</v>
+      </c>
+      <c r="S6" s="74"/>
       <c r="T6" s="67"/>
-      <c r="U6" s="90" t="s">
+      <c r="U6" s="99" t="s">
         <v>18</v>
       </c>
       <c r="V6" s="3" t="s">
@@ -7906,286 +7979,330 @@
       <c r="W6" s="67"/>
     </row>
     <row r="7" spans="1:23" s="11" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="3">
+      <c r="A7" s="74">
         <v>2</v>
       </c>
       <c r="B7" s="59">
         <v>44861</v>
       </c>
       <c r="C7" s="59"/>
-      <c r="D7" s="57" t="s">
+      <c r="D7" s="60" t="s">
         <v>68</v>
       </c>
-      <c r="E7" s="58">
+      <c r="E7" s="73">
         <v>868926033918407</v>
       </c>
-      <c r="F7" s="57"/>
-      <c r="G7" s="57" t="s">
+      <c r="F7" s="60"/>
+      <c r="G7" s="60" t="s">
         <v>63</v>
       </c>
-      <c r="H7" s="37"/>
-      <c r="I7" s="51"/>
-      <c r="J7" s="1"/>
-      <c r="K7" s="55"/>
-      <c r="L7" s="39"/>
-      <c r="M7" s="39"/>
-      <c r="N7" s="1"/>
-      <c r="O7" s="1"/>
-      <c r="P7" s="39"/>
-      <c r="Q7" s="1"/>
-      <c r="R7" s="2"/>
-      <c r="S7" s="3"/>
+      <c r="H7" s="60"/>
+      <c r="I7" s="61" t="s">
+        <v>87</v>
+      </c>
+      <c r="J7" s="62" t="s">
+        <v>109</v>
+      </c>
+      <c r="K7" s="63"/>
+      <c r="L7" s="64" t="s">
+        <v>102</v>
+      </c>
+      <c r="M7" s="64" t="s">
+        <v>110</v>
+      </c>
+      <c r="N7" s="62"/>
+      <c r="O7" s="62" t="s">
+        <v>77</v>
+      </c>
+      <c r="P7" s="64" t="s">
+        <v>78</v>
+      </c>
+      <c r="Q7" s="62" t="s">
+        <v>100</v>
+      </c>
+      <c r="R7" s="65" t="s">
+        <v>111</v>
+      </c>
+      <c r="S7" s="74"/>
       <c r="T7" s="67"/>
-      <c r="U7" s="91"/>
+      <c r="U7" s="100"/>
       <c r="V7" s="3" t="s">
         <v>35</v>
       </c>
       <c r="W7" s="67"/>
     </row>
     <row r="8" spans="1:23" s="11" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="3">
+      <c r="A8" s="74">
         <v>3</v>
       </c>
       <c r="B8" s="59">
         <v>44861</v>
       </c>
       <c r="C8" s="59"/>
-      <c r="D8" s="57" t="s">
+      <c r="D8" s="60" t="s">
         <v>68</v>
       </c>
-      <c r="E8" s="58">
+      <c r="E8" s="73">
         <v>868926033936144</v>
       </c>
-      <c r="F8" s="57" t="s">
+      <c r="F8" s="60" t="s">
         <v>67</v>
       </c>
-      <c r="G8" s="57" t="s">
+      <c r="G8" s="60" t="s">
         <v>63</v>
       </c>
-      <c r="H8" s="37"/>
-      <c r="I8" s="51" t="s">
+      <c r="H8" s="60"/>
+      <c r="I8" s="61" t="s">
         <v>106</v>
       </c>
-      <c r="J8" s="1"/>
-      <c r="K8" s="55" t="s">
+      <c r="J8" s="62"/>
+      <c r="K8" s="63" t="s">
         <v>102</v>
       </c>
-      <c r="L8" s="39"/>
-      <c r="M8" s="39"/>
-      <c r="N8" s="1"/>
-      <c r="O8" s="1"/>
-      <c r="P8" s="39"/>
-      <c r="Q8" s="1"/>
-      <c r="R8" s="2"/>
-      <c r="S8" s="3"/>
+      <c r="L8" s="64"/>
+      <c r="M8" s="64" t="s">
+        <v>89</v>
+      </c>
+      <c r="N8" s="62"/>
+      <c r="O8" s="62" t="s">
+        <v>77</v>
+      </c>
+      <c r="P8" s="64" t="s">
+        <v>78</v>
+      </c>
+      <c r="Q8" s="62" t="s">
+        <v>19</v>
+      </c>
+      <c r="R8" s="65" t="s">
+        <v>25</v>
+      </c>
+      <c r="S8" s="74"/>
       <c r="T8" s="67"/>
-      <c r="U8" s="91"/>
+      <c r="U8" s="100"/>
       <c r="V8" s="3" t="s">
         <v>21</v>
       </c>
       <c r="W8" s="67"/>
     </row>
     <row r="9" spans="1:23" s="11" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="3">
+      <c r="A9" s="74">
         <v>4</v>
       </c>
       <c r="B9" s="59">
         <v>44861</v>
       </c>
       <c r="C9" s="59"/>
-      <c r="D9" s="57" t="s">
+      <c r="D9" s="60" t="s">
         <v>68</v>
       </c>
-      <c r="E9" s="58">
+      <c r="E9" s="73">
         <v>864811036929946</v>
       </c>
-      <c r="F9" s="57" t="s">
+      <c r="F9" s="60" t="s">
         <v>67</v>
       </c>
-      <c r="G9" s="57" t="s">
+      <c r="G9" s="60" t="s">
         <v>63</v>
       </c>
-      <c r="H9" s="37" t="s">
+      <c r="H9" s="60" t="s">
         <v>105</v>
       </c>
-      <c r="I9" s="51" t="s">
+      <c r="I9" s="61" t="s">
         <v>87</v>
       </c>
-      <c r="J9" s="1"/>
-      <c r="K9" s="1" t="s">
+      <c r="J9" s="62"/>
+      <c r="K9" s="62" t="s">
         <v>102</v>
       </c>
-      <c r="L9" s="1"/>
-      <c r="M9" s="39" t="s">
+      <c r="L9" s="62"/>
+      <c r="M9" s="64" t="s">
         <v>89</v>
       </c>
-      <c r="N9" s="1"/>
-      <c r="O9" s="1" t="s">
+      <c r="N9" s="62"/>
+      <c r="O9" s="62" t="s">
         <v>77</v>
       </c>
-      <c r="P9" s="39" t="s">
+      <c r="P9" s="64" t="s">
         <v>78</v>
       </c>
-      <c r="Q9" s="1" t="s">
+      <c r="Q9" s="62" t="s">
         <v>19</v>
       </c>
-      <c r="R9" s="2" t="s">
+      <c r="R9" s="65" t="s">
         <v>25</v>
       </c>
-      <c r="S9" s="3"/>
+      <c r="S9" s="74"/>
       <c r="T9" s="67"/>
-      <c r="U9" s="91"/>
+      <c r="U9" s="100"/>
       <c r="V9" s="3" t="s">
         <v>51</v>
       </c>
       <c r="W9" s="67"/>
     </row>
     <row r="10" spans="1:23" s="11" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="3">
+      <c r="A10" s="74">
         <v>5</v>
       </c>
       <c r="B10" s="59">
         <v>44861</v>
       </c>
       <c r="C10" s="59"/>
-      <c r="D10" s="57" t="s">
+      <c r="D10" s="60" t="s">
         <v>68</v>
       </c>
-      <c r="E10" s="58">
+      <c r="E10" s="73">
         <v>864811037229346</v>
       </c>
-      <c r="F10" s="57" t="s">
+      <c r="F10" s="60" t="s">
         <v>67</v>
       </c>
-      <c r="G10" s="57" t="s">
+      <c r="G10" s="60" t="s">
         <v>63</v>
       </c>
-      <c r="H10" s="56" t="s">
+      <c r="H10" s="75" t="s">
         <v>104</v>
       </c>
-      <c r="I10" s="51" t="s">
+      <c r="I10" s="61" t="s">
         <v>87</v>
       </c>
-      <c r="J10" s="1" t="s">
+      <c r="J10" s="62" t="s">
         <v>88</v>
       </c>
-      <c r="K10" s="38" t="s">
+      <c r="K10" s="73" t="s">
         <v>103</v>
       </c>
-      <c r="L10" s="39"/>
-      <c r="M10" s="39" t="s">
+      <c r="L10" s="64"/>
+      <c r="M10" s="64" t="s">
         <v>89</v>
       </c>
-      <c r="N10" s="1"/>
-      <c r="O10" s="1" t="s">
+      <c r="N10" s="62"/>
+      <c r="O10" s="62" t="s">
         <v>77</v>
       </c>
-      <c r="P10" s="39" t="s">
+      <c r="P10" s="64" t="s">
         <v>78</v>
       </c>
-      <c r="Q10" s="1" t="s">
+      <c r="Q10" s="62" t="s">
         <v>19</v>
       </c>
-      <c r="R10" s="2" t="s">
+      <c r="R10" s="65" t="s">
         <v>25</v>
       </c>
-      <c r="S10" s="3"/>
+      <c r="S10" s="74"/>
       <c r="T10" s="67"/>
-      <c r="U10" s="91"/>
+      <c r="U10" s="100"/>
       <c r="V10" s="3" t="s">
         <v>31</v>
       </c>
       <c r="W10" s="67"/>
     </row>
     <row r="11" spans="1:23" s="11" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="3">
+      <c r="A11" s="74">
         <v>6</v>
       </c>
       <c r="B11" s="59">
         <v>44861</v>
       </c>
       <c r="C11" s="59"/>
-      <c r="D11" s="57" t="s">
+      <c r="D11" s="60" t="s">
         <v>68</v>
       </c>
-      <c r="E11" s="58">
+      <c r="E11" s="73">
         <v>868926033906766</v>
       </c>
-      <c r="F11" s="57"/>
-      <c r="G11" s="57" t="s">
+      <c r="F11" s="60"/>
+      <c r="G11" s="60" t="s">
         <v>63</v>
       </c>
-      <c r="H11" s="56" t="s">
+      <c r="H11" s="75" t="s">
         <v>91</v>
       </c>
-      <c r="I11" s="51" t="s">
+      <c r="I11" s="61" t="s">
         <v>97</v>
       </c>
-      <c r="J11" s="1" t="s">
+      <c r="J11" s="62" t="s">
         <v>98</v>
       </c>
-      <c r="K11" s="38" t="s">
+      <c r="K11" s="73" t="s">
         <v>96</v>
       </c>
-      <c r="L11" s="1" t="s">
+      <c r="L11" s="62" t="s">
         <v>102</v>
       </c>
-      <c r="M11" s="39" t="s">
+      <c r="M11" s="64" t="s">
         <v>99</v>
       </c>
-      <c r="N11" s="1"/>
-      <c r="O11" s="1" t="s">
+      <c r="N11" s="62"/>
+      <c r="O11" s="62" t="s">
         <v>77</v>
       </c>
-      <c r="P11" s="39" t="s">
+      <c r="P11" s="64" t="s">
         <v>78</v>
       </c>
-      <c r="Q11" s="1" t="s">
+      <c r="Q11" s="62" t="s">
         <v>100</v>
       </c>
-      <c r="R11" s="2" t="s">
+      <c r="R11" s="65" t="s">
         <v>101</v>
       </c>
-      <c r="S11" s="3"/>
+      <c r="S11" s="74"/>
       <c r="T11" s="67"/>
-      <c r="U11" s="91"/>
+      <c r="U11" s="100"/>
       <c r="V11" s="3" t="s">
         <v>30</v>
       </c>
       <c r="W11" s="67"/>
     </row>
     <row r="12" spans="1:23" s="11" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="3">
+      <c r="A12" s="74">
         <v>7</v>
       </c>
       <c r="B12" s="59">
         <v>44861</v>
       </c>
       <c r="C12" s="59"/>
-      <c r="D12" s="57" t="s">
+      <c r="D12" s="60" t="s">
         <v>68</v>
       </c>
-      <c r="E12" s="58">
+      <c r="E12" s="73">
         <v>864811036926934</v>
       </c>
-      <c r="F12" s="57"/>
-      <c r="G12" s="57" t="s">
+      <c r="F12" s="60"/>
+      <c r="G12" s="60" t="s">
         <v>63</v>
       </c>
-      <c r="H12" s="56"/>
-      <c r="I12" s="51"/>
-      <c r="J12" s="1"/>
-      <c r="K12" s="1"/>
-      <c r="L12" s="1"/>
-      <c r="M12" s="39"/>
-      <c r="N12" s="1"/>
-      <c r="O12" s="1"/>
-      <c r="P12" s="39"/>
-      <c r="Q12" s="1"/>
-      <c r="R12" s="2"/>
-      <c r="S12" s="3"/>
+      <c r="H12" s="75"/>
+      <c r="I12" s="61" t="s">
+        <v>87</v>
+      </c>
+      <c r="J12" s="62" t="s">
+        <v>34</v>
+      </c>
+      <c r="K12" s="62"/>
+      <c r="L12" s="62" t="s">
+        <v>102</v>
+      </c>
+      <c r="M12" s="64" t="s">
+        <v>108</v>
+      </c>
+      <c r="N12" s="90">
+        <v>190000</v>
+      </c>
+      <c r="O12" s="62" t="s">
+        <v>77</v>
+      </c>
+      <c r="P12" s="64" t="s">
+        <v>78</v>
+      </c>
+      <c r="Q12" s="62" t="s">
+        <v>18</v>
+      </c>
+      <c r="R12" s="65" t="s">
+        <v>35</v>
+      </c>
+      <c r="S12" s="74"/>
       <c r="T12" s="67"/>
-      <c r="U12" s="90" t="s">
+      <c r="U12" s="99" t="s">
         <v>19</v>
       </c>
       <c r="V12" s="3" t="s">
@@ -8216,7 +8333,7 @@
       <c r="R13" s="2"/>
       <c r="S13" s="3"/>
       <c r="T13" s="67"/>
-      <c r="U13" s="91"/>
+      <c r="U13" s="100"/>
       <c r="V13" s="3" t="s">
         <v>37</v>
       </c>
@@ -8245,7 +8362,7 @@
       <c r="R14" s="2"/>
       <c r="S14" s="3"/>
       <c r="T14" s="67"/>
-      <c r="U14" s="91"/>
+      <c r="U14" s="100"/>
       <c r="V14" s="3" t="s">
         <v>36</v>
       </c>
@@ -8274,7 +8391,7 @@
       <c r="R15" s="2"/>
       <c r="S15" s="3"/>
       <c r="T15" s="13"/>
-      <c r="U15" s="91"/>
+      <c r="U15" s="100"/>
       <c r="V15" s="3" t="s">
         <v>24</v>
       </c>
@@ -8303,7 +8420,7 @@
       <c r="R16" s="2"/>
       <c r="S16" s="3"/>
       <c r="T16" s="13"/>
-      <c r="U16" s="92"/>
+      <c r="U16" s="101"/>
       <c r="V16" s="3" t="s">
         <v>25</v>
       </c>
@@ -8421,7 +8538,7 @@
       </c>
       <c r="V20" s="9">
         <f>COUNTIF($Q$6:$Q$51,"PM")</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="W20" s="13"/>
     </row>
@@ -8453,7 +8570,7 @@
       </c>
       <c r="V21" s="9">
         <f>COUNTIF($Q$6:$Q$51,"PC")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W21" s="13"/>
     </row>
@@ -8485,7 +8602,7 @@
       </c>
       <c r="V22" s="9">
         <f>COUNTIF($Q$6:$Q$51,"PC+PM")</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="W22" s="13"/>
     </row>
@@ -8634,7 +8751,7 @@
       </c>
       <c r="V27" s="9">
         <f>COUNTIF($R$6:$R$51,"*GSM*")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W27" s="13"/>
     </row>
@@ -8698,7 +8815,7 @@
       </c>
       <c r="V29" s="9">
         <f>COUNTIF($R$6:$R$51,"*NG*")</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="W29" s="13"/>
     </row>
@@ -8762,7 +8879,7 @@
       </c>
       <c r="V31" s="9">
         <f>COUNTIF($R$6:$R$51,"*LK*")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W31" s="13"/>
     </row>
@@ -8890,7 +9007,7 @@
       </c>
       <c r="V35" s="9">
         <f>COUNTIF($R$6:$R$51,"*NCFW*")</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="W35" s="13"/>
     </row>
@@ -8922,7 +9039,7 @@
       </c>
       <c r="V36" s="9">
         <f>COUNTIF($R$6:$R$51,"*KL*")</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="W36" s="13"/>
     </row>
@@ -8954,7 +9071,7 @@
       </c>
       <c r="V37" s="9">
         <f>SUM(V26:V36)</f>
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="W37" s="13"/>
     </row>
@@ -9307,7 +9424,7 @@
       <c r="S48" s="3"/>
       <c r="T48" s="34">
         <f>COUNTIF(J9:J20,"*GSM*")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U48" s="9" t="s">
         <v>57</v>
@@ -10019,6 +10136,13 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="U6:U11"/>
+    <mergeCell ref="U12:U16"/>
+    <mergeCell ref="P4:P5"/>
+    <mergeCell ref="Q4:Q5"/>
+    <mergeCell ref="R4:R5"/>
+    <mergeCell ref="S4:S5"/>
+    <mergeCell ref="U4:U5"/>
     <mergeCell ref="V4:V5"/>
     <mergeCell ref="A1:V1"/>
     <mergeCell ref="A2:D2"/>
@@ -10030,13 +10154,6 @@
     <mergeCell ref="M4:M5"/>
     <mergeCell ref="N4:N5"/>
     <mergeCell ref="O4:O5"/>
-    <mergeCell ref="U6:U11"/>
-    <mergeCell ref="U12:U16"/>
-    <mergeCell ref="P4:P5"/>
-    <mergeCell ref="Q4:Q5"/>
-    <mergeCell ref="R4:R5"/>
-    <mergeCell ref="S4:S5"/>
-    <mergeCell ref="U4:U5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -10048,7 +10165,7 @@
   <dimension ref="A1:X115"/>
   <sheetViews>
     <sheetView showZeros="0" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:F2"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -10080,41 +10197,41 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="99"/>
-      <c r="B1" s="99"/>
-      <c r="C1" s="99"/>
-      <c r="D1" s="99"/>
-      <c r="E1" s="99"/>
-      <c r="F1" s="99"/>
-      <c r="G1" s="99"/>
-      <c r="H1" s="99"/>
-      <c r="I1" s="99"/>
-      <c r="J1" s="99"/>
-      <c r="K1" s="99"/>
-      <c r="L1" s="99"/>
-      <c r="M1" s="99"/>
-      <c r="N1" s="99"/>
-      <c r="O1" s="99"/>
-      <c r="P1" s="99"/>
-      <c r="Q1" s="99"/>
-      <c r="R1" s="99"/>
-      <c r="S1" s="99"/>
-      <c r="T1" s="99"/>
-      <c r="U1" s="99"/>
-      <c r="V1" s="99"/>
+      <c r="A1" s="92"/>
+      <c r="B1" s="92"/>
+      <c r="C1" s="92"/>
+      <c r="D1" s="92"/>
+      <c r="E1" s="92"/>
+      <c r="F1" s="92"/>
+      <c r="G1" s="92"/>
+      <c r="H1" s="92"/>
+      <c r="I1" s="92"/>
+      <c r="J1" s="92"/>
+      <c r="K1" s="92"/>
+      <c r="L1" s="92"/>
+      <c r="M1" s="92"/>
+      <c r="N1" s="92"/>
+      <c r="O1" s="92"/>
+      <c r="P1" s="92"/>
+      <c r="Q1" s="92"/>
+      <c r="R1" s="92"/>
+      <c r="S1" s="92"/>
+      <c r="T1" s="92"/>
+      <c r="U1" s="92"/>
+      <c r="V1" s="92"/>
       <c r="W1" s="44"/>
     </row>
     <row r="2" spans="1:23" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="100" t="s">
+      <c r="A2" s="93" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="101"/>
-      <c r="C2" s="101"/>
-      <c r="D2" s="101"/>
-      <c r="E2" s="104" t="s">
+      <c r="B2" s="94"/>
+      <c r="C2" s="94"/>
+      <c r="D2" s="94"/>
+      <c r="E2" s="105" t="s">
         <v>64</v>
       </c>
-      <c r="F2" s="104"/>
+      <c r="F2" s="105"/>
       <c r="G2" s="4"/>
       <c r="H2" s="20"/>
       <c r="I2" s="48"/>
@@ -10159,58 +10276,58 @@
       <c r="W3" s="26"/>
     </row>
     <row r="4" spans="1:23" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="103" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" s="98" t="s">
+      <c r="A4" s="96" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="91" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="98"/>
-      <c r="D4" s="98"/>
-      <c r="E4" s="98"/>
-      <c r="F4" s="98"/>
-      <c r="G4" s="98"/>
-      <c r="H4" s="98"/>
-      <c r="I4" s="98"/>
-      <c r="J4" s="98" t="s">
+      <c r="C4" s="91"/>
+      <c r="D4" s="91"/>
+      <c r="E4" s="91"/>
+      <c r="F4" s="91"/>
+      <c r="G4" s="91"/>
+      <c r="H4" s="91"/>
+      <c r="I4" s="91"/>
+      <c r="J4" s="91" t="s">
         <v>6</v>
       </c>
-      <c r="K4" s="98" t="s">
+      <c r="K4" s="91" t="s">
         <v>11</v>
       </c>
-      <c r="L4" s="98"/>
-      <c r="M4" s="95" t="s">
+      <c r="L4" s="91"/>
+      <c r="M4" s="97" t="s">
         <v>42</v>
       </c>
-      <c r="N4" s="95" t="s">
+      <c r="N4" s="97" t="s">
         <v>10</v>
       </c>
-      <c r="O4" s="95" t="s">
+      <c r="O4" s="97" t="s">
         <v>7</v>
       </c>
-      <c r="P4" s="93" t="s">
+      <c r="P4" s="102" t="s">
         <v>14</v>
       </c>
-      <c r="Q4" s="95" t="s">
+      <c r="Q4" s="97" t="s">
         <v>39</v>
       </c>
-      <c r="R4" s="95" t="s">
+      <c r="R4" s="97" t="s">
         <v>53</v>
       </c>
-      <c r="S4" s="97" t="s">
+      <c r="S4" s="104" t="s">
         <v>54</v>
       </c>
       <c r="T4" s="26"/>
-      <c r="U4" s="98" t="s">
+      <c r="U4" s="91" t="s">
         <v>39</v>
       </c>
-      <c r="V4" s="98" t="s">
+      <c r="V4" s="91" t="s">
         <v>53</v>
       </c>
       <c r="W4" s="45"/>
     </row>
     <row r="5" spans="1:23" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="103"/>
+      <c r="A5" s="96"/>
       <c r="B5" s="77" t="s">
         <v>1</v>
       </c>
@@ -10235,23 +10352,23 @@
       <c r="I5" s="50" t="s">
         <v>15</v>
       </c>
-      <c r="J5" s="98"/>
+      <c r="J5" s="91"/>
       <c r="K5" s="77" t="s">
         <v>12</v>
       </c>
       <c r="L5" s="77" t="s">
         <v>13</v>
       </c>
-      <c r="M5" s="96"/>
-      <c r="N5" s="96"/>
-      <c r="O5" s="96"/>
-      <c r="P5" s="94"/>
-      <c r="Q5" s="96"/>
-      <c r="R5" s="96"/>
-      <c r="S5" s="97"/>
+      <c r="M5" s="98"/>
+      <c r="N5" s="98"/>
+      <c r="O5" s="98"/>
+      <c r="P5" s="103"/>
+      <c r="Q5" s="98"/>
+      <c r="R5" s="98"/>
+      <c r="S5" s="104"/>
       <c r="T5" s="26"/>
-      <c r="U5" s="98"/>
-      <c r="V5" s="98"/>
+      <c r="U5" s="91"/>
+      <c r="V5" s="91"/>
       <c r="W5" s="45"/>
     </row>
     <row r="6" spans="1:23" s="11" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -10273,9 +10390,13 @@
         <v>63</v>
       </c>
       <c r="H6" s="60"/>
-      <c r="I6" s="61"/>
+      <c r="I6" s="61" t="s">
+        <v>87</v>
+      </c>
       <c r="J6" s="62"/>
-      <c r="K6" s="63"/>
+      <c r="K6" s="63" t="s">
+        <v>116</v>
+      </c>
       <c r="L6" s="64"/>
       <c r="M6" s="64"/>
       <c r="N6" s="62"/>
@@ -10285,7 +10406,7 @@
       <c r="R6" s="65"/>
       <c r="S6" s="3"/>
       <c r="T6" s="76"/>
-      <c r="U6" s="90" t="s">
+      <c r="U6" s="99" t="s">
         <v>18</v>
       </c>
       <c r="V6" s="3" t="s">
@@ -10311,20 +10432,38 @@
       <c r="G7" s="57" t="s">
         <v>63</v>
       </c>
-      <c r="H7" s="37"/>
-      <c r="I7" s="61"/>
-      <c r="J7" s="1"/>
-      <c r="K7" s="55"/>
+      <c r="H7" s="60" t="s">
+        <v>91</v>
+      </c>
+      <c r="I7" s="61" t="s">
+        <v>87</v>
+      </c>
+      <c r="J7" s="62" t="s">
+        <v>109</v>
+      </c>
+      <c r="K7" s="63" t="s">
+        <v>112</v>
+      </c>
       <c r="L7" s="63"/>
-      <c r="M7" s="39"/>
+      <c r="M7" s="39" t="s">
+        <v>113</v>
+      </c>
       <c r="N7" s="1"/>
-      <c r="O7" s="1"/>
-      <c r="P7" s="39"/>
-      <c r="Q7" s="1"/>
-      <c r="R7" s="2"/>
+      <c r="O7" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="P7" s="39" t="s">
+        <v>78</v>
+      </c>
+      <c r="Q7" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="R7" s="2" t="s">
+        <v>24</v>
+      </c>
       <c r="S7" s="3"/>
       <c r="T7" s="76"/>
-      <c r="U7" s="91"/>
+      <c r="U7" s="100"/>
       <c r="V7" s="3" t="s">
         <v>35</v>
       </c>
@@ -10344,24 +10483,44 @@
       <c r="E8" s="58">
         <v>863586032923637</v>
       </c>
-      <c r="F8" s="57"/>
+      <c r="F8" s="57" t="s">
+        <v>67</v>
+      </c>
       <c r="G8" s="57" t="s">
         <v>63</v>
       </c>
-      <c r="H8" s="37"/>
-      <c r="I8" s="61"/>
-      <c r="J8" s="1"/>
-      <c r="K8" s="55"/>
-      <c r="L8" s="63"/>
-      <c r="M8" s="39"/>
+      <c r="H8" s="60" t="s">
+        <v>90</v>
+      </c>
+      <c r="I8" s="61" t="s">
+        <v>106</v>
+      </c>
+      <c r="J8" s="62" t="s">
+        <v>114</v>
+      </c>
+      <c r="K8" s="63"/>
+      <c r="L8" s="63" t="s">
+        <v>112</v>
+      </c>
+      <c r="M8" s="39" t="s">
+        <v>115</v>
+      </c>
       <c r="N8" s="1"/>
-      <c r="O8" s="1"/>
-      <c r="P8" s="39"/>
-      <c r="Q8" s="1"/>
-      <c r="R8" s="2"/>
+      <c r="O8" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="P8" s="39" t="s">
+        <v>78</v>
+      </c>
+      <c r="Q8" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="R8" s="2" t="s">
+        <v>30</v>
+      </c>
       <c r="S8" s="3"/>
       <c r="T8" s="76"/>
-      <c r="U8" s="91"/>
+      <c r="U8" s="100"/>
       <c r="V8" s="3" t="s">
         <v>21</v>
       </c>
@@ -10390,7 +10549,7 @@
       <c r="R9" s="2"/>
       <c r="S9" s="3"/>
       <c r="T9" s="76"/>
-      <c r="U9" s="91"/>
+      <c r="U9" s="100"/>
       <c r="V9" s="3" t="s">
         <v>51</v>
       </c>
@@ -10419,7 +10578,7 @@
       <c r="R10" s="2"/>
       <c r="S10" s="3"/>
       <c r="T10" s="76"/>
-      <c r="U10" s="91"/>
+      <c r="U10" s="100"/>
       <c r="V10" s="3" t="s">
         <v>31</v>
       </c>
@@ -10448,7 +10607,7 @@
       <c r="R11" s="2"/>
       <c r="S11" s="3"/>
       <c r="T11" s="76"/>
-      <c r="U11" s="91"/>
+      <c r="U11" s="100"/>
       <c r="V11" s="3" t="s">
         <v>30</v>
       </c>
@@ -10477,7 +10636,7 @@
       <c r="R12" s="2"/>
       <c r="S12" s="3"/>
       <c r="T12" s="76"/>
-      <c r="U12" s="90" t="s">
+      <c r="U12" s="99" t="s">
         <v>19</v>
       </c>
       <c r="V12" s="3" t="s">
@@ -10508,7 +10667,7 @@
       <c r="R13" s="2"/>
       <c r="S13" s="3"/>
       <c r="T13" s="76"/>
-      <c r="U13" s="91"/>
+      <c r="U13" s="100"/>
       <c r="V13" s="3" t="s">
         <v>37</v>
       </c>
@@ -10537,7 +10696,7 @@
       <c r="R14" s="2"/>
       <c r="S14" s="3"/>
       <c r="T14" s="76"/>
-      <c r="U14" s="91"/>
+      <c r="U14" s="100"/>
       <c r="V14" s="3" t="s">
         <v>36</v>
       </c>
@@ -10566,7 +10725,7 @@
       <c r="R15" s="2"/>
       <c r="S15" s="3"/>
       <c r="T15" s="13"/>
-      <c r="U15" s="91"/>
+      <c r="U15" s="100"/>
       <c r="V15" s="3" t="s">
         <v>24</v>
       </c>
@@ -10595,7 +10754,7 @@
       <c r="R16" s="2"/>
       <c r="S16" s="3"/>
       <c r="T16" s="13"/>
-      <c r="U16" s="92"/>
+      <c r="U16" s="101"/>
       <c r="V16" s="3" t="s">
         <v>25</v>
       </c>
@@ -10713,7 +10872,7 @@
       </c>
       <c r="V20" s="9">
         <f>COUNTIF($Q$6:$Q$51,"PM")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W20" s="13"/>
     </row>
@@ -10745,7 +10904,7 @@
       </c>
       <c r="V21" s="9">
         <f>COUNTIF($Q$6:$Q$51,"PC")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W21" s="13"/>
     </row>
@@ -11054,7 +11213,7 @@
       </c>
       <c r="V31" s="9">
         <f>COUNTIF($R$6:$R$51,"*LK*")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W31" s="13"/>
     </row>
@@ -11182,7 +11341,7 @@
       </c>
       <c r="V35" s="9">
         <f>COUNTIF($R$6:$R$51,"*NCFW*")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W35" s="13"/>
     </row>
@@ -11246,7 +11405,7 @@
       </c>
       <c r="V37" s="9">
         <f>SUM(V26:V36)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="W37" s="13"/>
     </row>
@@ -12311,6 +12470,13 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="U6:U11"/>
+    <mergeCell ref="U12:U16"/>
+    <mergeCell ref="P4:P5"/>
+    <mergeCell ref="Q4:Q5"/>
+    <mergeCell ref="R4:R5"/>
+    <mergeCell ref="S4:S5"/>
+    <mergeCell ref="U4:U5"/>
     <mergeCell ref="V4:V5"/>
     <mergeCell ref="A1:V1"/>
     <mergeCell ref="A2:D2"/>
@@ -12322,13 +12488,6 @@
     <mergeCell ref="M4:M5"/>
     <mergeCell ref="N4:N5"/>
     <mergeCell ref="O4:O5"/>
-    <mergeCell ref="U6:U11"/>
-    <mergeCell ref="U12:U16"/>
-    <mergeCell ref="P4:P5"/>
-    <mergeCell ref="Q4:Q5"/>
-    <mergeCell ref="R4:R5"/>
-    <mergeCell ref="S4:S5"/>
-    <mergeCell ref="U4:U5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -12339,8 +12498,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X115"/>
   <sheetViews>
-    <sheetView showZeros="0" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:F2"/>
+    <sheetView showZeros="0" topLeftCell="L1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="S7" sqref="S7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -12372,41 +12531,41 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="99"/>
-      <c r="B1" s="99"/>
-      <c r="C1" s="99"/>
-      <c r="D1" s="99"/>
-      <c r="E1" s="99"/>
-      <c r="F1" s="99"/>
-      <c r="G1" s="99"/>
-      <c r="H1" s="99"/>
-      <c r="I1" s="99"/>
-      <c r="J1" s="99"/>
-      <c r="K1" s="99"/>
-      <c r="L1" s="99"/>
-      <c r="M1" s="99"/>
-      <c r="N1" s="99"/>
-      <c r="O1" s="99"/>
-      <c r="P1" s="99"/>
-      <c r="Q1" s="99"/>
-      <c r="R1" s="99"/>
-      <c r="S1" s="99"/>
-      <c r="T1" s="99"/>
-      <c r="U1" s="99"/>
-      <c r="V1" s="99"/>
+      <c r="A1" s="92"/>
+      <c r="B1" s="92"/>
+      <c r="C1" s="92"/>
+      <c r="D1" s="92"/>
+      <c r="E1" s="92"/>
+      <c r="F1" s="92"/>
+      <c r="G1" s="92"/>
+      <c r="H1" s="92"/>
+      <c r="I1" s="92"/>
+      <c r="J1" s="92"/>
+      <c r="K1" s="92"/>
+      <c r="L1" s="92"/>
+      <c r="M1" s="92"/>
+      <c r="N1" s="92"/>
+      <c r="O1" s="92"/>
+      <c r="P1" s="92"/>
+      <c r="Q1" s="92"/>
+      <c r="R1" s="92"/>
+      <c r="S1" s="92"/>
+      <c r="T1" s="92"/>
+      <c r="U1" s="92"/>
+      <c r="V1" s="92"/>
       <c r="W1" s="44"/>
     </row>
     <row r="2" spans="1:23" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="100" t="s">
+      <c r="A2" s="93" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="101"/>
-      <c r="C2" s="101"/>
-      <c r="D2" s="101"/>
-      <c r="E2" s="104" t="s">
+      <c r="B2" s="94"/>
+      <c r="C2" s="94"/>
+      <c r="D2" s="94"/>
+      <c r="E2" s="105" t="s">
         <v>64</v>
       </c>
-      <c r="F2" s="104"/>
+      <c r="F2" s="105"/>
       <c r="G2" s="4"/>
       <c r="H2" s="20"/>
       <c r="I2" s="48"/>
@@ -12451,58 +12610,58 @@
       <c r="W3" s="26"/>
     </row>
     <row r="4" spans="1:23" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="103" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" s="98" t="s">
+      <c r="A4" s="96" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="91" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="98"/>
-      <c r="D4" s="98"/>
-      <c r="E4" s="98"/>
-      <c r="F4" s="98"/>
-      <c r="G4" s="98"/>
-      <c r="H4" s="98"/>
-      <c r="I4" s="98"/>
-      <c r="J4" s="98" t="s">
+      <c r="C4" s="91"/>
+      <c r="D4" s="91"/>
+      <c r="E4" s="91"/>
+      <c r="F4" s="91"/>
+      <c r="G4" s="91"/>
+      <c r="H4" s="91"/>
+      <c r="I4" s="91"/>
+      <c r="J4" s="91" t="s">
         <v>6</v>
       </c>
-      <c r="K4" s="98" t="s">
+      <c r="K4" s="91" t="s">
         <v>11</v>
       </c>
-      <c r="L4" s="98"/>
-      <c r="M4" s="95" t="s">
+      <c r="L4" s="91"/>
+      <c r="M4" s="97" t="s">
         <v>42</v>
       </c>
-      <c r="N4" s="95" t="s">
+      <c r="N4" s="97" t="s">
         <v>10</v>
       </c>
-      <c r="O4" s="95" t="s">
+      <c r="O4" s="97" t="s">
         <v>7</v>
       </c>
-      <c r="P4" s="93" t="s">
+      <c r="P4" s="102" t="s">
         <v>14</v>
       </c>
-      <c r="Q4" s="95" t="s">
+      <c r="Q4" s="97" t="s">
         <v>39</v>
       </c>
-      <c r="R4" s="95" t="s">
+      <c r="R4" s="97" t="s">
         <v>53</v>
       </c>
-      <c r="S4" s="97" t="s">
+      <c r="S4" s="104" t="s">
         <v>54</v>
       </c>
       <c r="T4" s="26"/>
-      <c r="U4" s="98" t="s">
+      <c r="U4" s="91" t="s">
         <v>39</v>
       </c>
-      <c r="V4" s="98" t="s">
+      <c r="V4" s="91" t="s">
         <v>53</v>
       </c>
       <c r="W4" s="45"/>
     </row>
     <row r="5" spans="1:23" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="103"/>
+      <c r="A5" s="96"/>
       <c r="B5" s="66" t="s">
         <v>1</v>
       </c>
@@ -12527,23 +12686,23 @@
       <c r="I5" s="50" t="s">
         <v>15</v>
       </c>
-      <c r="J5" s="98"/>
+      <c r="J5" s="91"/>
       <c r="K5" s="66" t="s">
         <v>12</v>
       </c>
       <c r="L5" s="66" t="s">
         <v>13</v>
       </c>
-      <c r="M5" s="96"/>
-      <c r="N5" s="96"/>
-      <c r="O5" s="96"/>
-      <c r="P5" s="94"/>
-      <c r="Q5" s="96"/>
-      <c r="R5" s="96"/>
-      <c r="S5" s="97"/>
+      <c r="M5" s="98"/>
+      <c r="N5" s="98"/>
+      <c r="O5" s="98"/>
+      <c r="P5" s="103"/>
+      <c r="Q5" s="98"/>
+      <c r="R5" s="98"/>
+      <c r="S5" s="104"/>
       <c r="T5" s="26"/>
-      <c r="U5" s="98"/>
-      <c r="V5" s="98"/>
+      <c r="U5" s="91"/>
+      <c r="V5" s="91"/>
       <c r="W5" s="45"/>
     </row>
     <row r="6" spans="1:23" s="11" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -12565,19 +12724,37 @@
         <v>63</v>
       </c>
       <c r="H6" s="60"/>
-      <c r="I6" s="61"/>
-      <c r="J6" s="62"/>
-      <c r="K6" s="63"/>
-      <c r="L6" s="64"/>
-      <c r="M6" s="64"/>
+      <c r="I6" s="61" t="s">
+        <v>121</v>
+      </c>
+      <c r="J6" s="62" t="s">
+        <v>122</v>
+      </c>
+      <c r="K6" s="63" t="s">
+        <v>120</v>
+      </c>
+      <c r="L6" s="55" t="s">
+        <v>117</v>
+      </c>
+      <c r="M6" s="64" t="s">
+        <v>38</v>
+      </c>
       <c r="N6" s="62"/>
-      <c r="O6" s="62"/>
-      <c r="P6" s="64"/>
-      <c r="Q6" s="62"/>
-      <c r="R6" s="65"/>
+      <c r="O6" s="62" t="s">
+        <v>77</v>
+      </c>
+      <c r="P6" s="64" t="s">
+        <v>78</v>
+      </c>
+      <c r="Q6" s="62" t="s">
+        <v>19</v>
+      </c>
+      <c r="R6" s="65" t="s">
+        <v>24</v>
+      </c>
       <c r="S6" s="3"/>
       <c r="T6" s="67"/>
-      <c r="U6" s="90" t="s">
+      <c r="U6" s="99" t="s">
         <v>18</v>
       </c>
       <c r="V6" s="3" t="s">
@@ -12603,20 +12780,38 @@
       <c r="G7" s="57" t="s">
         <v>63</v>
       </c>
-      <c r="H7" s="37"/>
-      <c r="I7" s="61"/>
-      <c r="J7" s="1"/>
+      <c r="H7" s="60" t="s">
+        <v>124</v>
+      </c>
+      <c r="I7" s="61" t="s">
+        <v>87</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>84</v>
+      </c>
       <c r="K7" s="55"/>
-      <c r="L7" s="63"/>
-      <c r="M7" s="39"/>
+      <c r="L7" s="55" t="s">
+        <v>117</v>
+      </c>
+      <c r="M7" s="39" t="s">
+        <v>123</v>
+      </c>
       <c r="N7" s="1"/>
-      <c r="O7" s="1"/>
-      <c r="P7" s="39"/>
-      <c r="Q7" s="1"/>
-      <c r="R7" s="2"/>
+      <c r="O7" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="P7" s="39" t="s">
+        <v>78</v>
+      </c>
+      <c r="Q7" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="R7" s="2" t="s">
+        <v>24</v>
+      </c>
       <c r="S7" s="3"/>
       <c r="T7" s="67"/>
-      <c r="U7" s="91"/>
+      <c r="U7" s="100"/>
       <c r="V7" s="3" t="s">
         <v>35</v>
       </c>
@@ -12641,19 +12836,35 @@
         <v>63</v>
       </c>
       <c r="H8" s="37"/>
-      <c r="I8" s="61"/>
-      <c r="J8" s="1"/>
-      <c r="K8" s="55"/>
+      <c r="I8" s="61" t="s">
+        <v>87</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="K8" s="55" t="s">
+        <v>117</v>
+      </c>
       <c r="L8" s="63"/>
-      <c r="M8" s="39"/>
+      <c r="M8" s="39" t="s">
+        <v>119</v>
+      </c>
       <c r="N8" s="1"/>
-      <c r="O8" s="1"/>
-      <c r="P8" s="39"/>
-      <c r="Q8" s="1"/>
-      <c r="R8" s="2"/>
+      <c r="O8" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="P8" s="39" t="s">
+        <v>78</v>
+      </c>
+      <c r="Q8" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="R8" s="2" t="s">
+        <v>30</v>
+      </c>
       <c r="S8" s="3"/>
       <c r="T8" s="67"/>
-      <c r="U8" s="91"/>
+      <c r="U8" s="100"/>
       <c r="V8" s="3" t="s">
         <v>21</v>
       </c>
@@ -12682,7 +12893,7 @@
       <c r="R9" s="2"/>
       <c r="S9" s="3"/>
       <c r="T9" s="67"/>
-      <c r="U9" s="91"/>
+      <c r="U9" s="100"/>
       <c r="V9" s="3" t="s">
         <v>51</v>
       </c>
@@ -12711,7 +12922,7 @@
       <c r="R10" s="2"/>
       <c r="S10" s="3"/>
       <c r="T10" s="67"/>
-      <c r="U10" s="91"/>
+      <c r="U10" s="100"/>
       <c r="V10" s="3" t="s">
         <v>31</v>
       </c>
@@ -12740,7 +12951,7 @@
       <c r="R11" s="2"/>
       <c r="S11" s="3"/>
       <c r="T11" s="67"/>
-      <c r="U11" s="91"/>
+      <c r="U11" s="100"/>
       <c r="V11" s="3" t="s">
         <v>30</v>
       </c>
@@ -12769,7 +12980,7 @@
       <c r="R12" s="2"/>
       <c r="S12" s="3"/>
       <c r="T12" s="67"/>
-      <c r="U12" s="90" t="s">
+      <c r="U12" s="99" t="s">
         <v>19</v>
       </c>
       <c r="V12" s="3" t="s">
@@ -12800,7 +13011,7 @@
       <c r="R13" s="2"/>
       <c r="S13" s="3"/>
       <c r="T13" s="67"/>
-      <c r="U13" s="91"/>
+      <c r="U13" s="100"/>
       <c r="V13" s="3" t="s">
         <v>37</v>
       </c>
@@ -12829,7 +13040,7 @@
       <c r="R14" s="2"/>
       <c r="S14" s="3"/>
       <c r="T14" s="67"/>
-      <c r="U14" s="91"/>
+      <c r="U14" s="100"/>
       <c r="V14" s="3" t="s">
         <v>36</v>
       </c>
@@ -12858,7 +13069,7 @@
       <c r="R15" s="2"/>
       <c r="S15" s="3"/>
       <c r="T15" s="13"/>
-      <c r="U15" s="91"/>
+      <c r="U15" s="100"/>
       <c r="V15" s="3" t="s">
         <v>24</v>
       </c>
@@ -12887,7 +13098,7 @@
       <c r="R16" s="2"/>
       <c r="S16" s="3"/>
       <c r="T16" s="13"/>
-      <c r="U16" s="92"/>
+      <c r="U16" s="101"/>
       <c r="V16" s="3" t="s">
         <v>25</v>
       </c>
@@ -13005,7 +13216,7 @@
       </c>
       <c r="V20" s="9">
         <f>COUNTIF($Q$6:$Q$51,"PM")</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="W20" s="13"/>
     </row>
@@ -13037,7 +13248,7 @@
       </c>
       <c r="V21" s="9">
         <f>COUNTIF($Q$6:$Q$51,"PC")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W21" s="13"/>
     </row>
@@ -13346,7 +13557,7 @@
       </c>
       <c r="V31" s="9">
         <f>COUNTIF($R$6:$R$51,"*LK*")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W31" s="13"/>
     </row>
@@ -13474,7 +13685,7 @@
       </c>
       <c r="V35" s="9">
         <f>COUNTIF($R$6:$R$51,"*NCFW*")</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="W35" s="13"/>
     </row>
@@ -13538,7 +13749,7 @@
       </c>
       <c r="V37" s="9">
         <f>SUM(V26:V36)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="W37" s="13"/>
     </row>
@@ -14603,6 +14814,13 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="U6:U11"/>
+    <mergeCell ref="U12:U16"/>
+    <mergeCell ref="P4:P5"/>
+    <mergeCell ref="Q4:Q5"/>
+    <mergeCell ref="R4:R5"/>
+    <mergeCell ref="S4:S5"/>
+    <mergeCell ref="U4:U5"/>
     <mergeCell ref="V4:V5"/>
     <mergeCell ref="A1:V1"/>
     <mergeCell ref="A2:D2"/>
@@ -14614,13 +14832,6 @@
     <mergeCell ref="M4:M5"/>
     <mergeCell ref="N4:N5"/>
     <mergeCell ref="O4:O5"/>
-    <mergeCell ref="U6:U11"/>
-    <mergeCell ref="U12:U16"/>
-    <mergeCell ref="P4:P5"/>
-    <mergeCell ref="Q4:Q5"/>
-    <mergeCell ref="R4:R5"/>
-    <mergeCell ref="S4:S5"/>
-    <mergeCell ref="U4:U5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -14664,41 +14875,41 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="99"/>
-      <c r="B1" s="99"/>
-      <c r="C1" s="99"/>
-      <c r="D1" s="99"/>
-      <c r="E1" s="99"/>
-      <c r="F1" s="99"/>
-      <c r="G1" s="99"/>
-      <c r="H1" s="99"/>
-      <c r="I1" s="99"/>
-      <c r="J1" s="99"/>
-      <c r="K1" s="99"/>
-      <c r="L1" s="99"/>
-      <c r="M1" s="99"/>
-      <c r="N1" s="99"/>
-      <c r="O1" s="99"/>
-      <c r="P1" s="99"/>
-      <c r="Q1" s="99"/>
-      <c r="R1" s="99"/>
-      <c r="S1" s="99"/>
-      <c r="T1" s="99"/>
-      <c r="U1" s="99"/>
-      <c r="V1" s="99"/>
+      <c r="A1" s="92"/>
+      <c r="B1" s="92"/>
+      <c r="C1" s="92"/>
+      <c r="D1" s="92"/>
+      <c r="E1" s="92"/>
+      <c r="F1" s="92"/>
+      <c r="G1" s="92"/>
+      <c r="H1" s="92"/>
+      <c r="I1" s="92"/>
+      <c r="J1" s="92"/>
+      <c r="K1" s="92"/>
+      <c r="L1" s="92"/>
+      <c r="M1" s="92"/>
+      <c r="N1" s="92"/>
+      <c r="O1" s="92"/>
+      <c r="P1" s="92"/>
+      <c r="Q1" s="92"/>
+      <c r="R1" s="92"/>
+      <c r="S1" s="92"/>
+      <c r="T1" s="92"/>
+      <c r="U1" s="92"/>
+      <c r="V1" s="92"/>
       <c r="W1" s="44"/>
     </row>
     <row r="2" spans="1:23" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="100" t="s">
+      <c r="A2" s="93" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="101"/>
-      <c r="C2" s="101"/>
-      <c r="D2" s="101"/>
-      <c r="E2" s="104" t="s">
+      <c r="B2" s="94"/>
+      <c r="C2" s="94"/>
+      <c r="D2" s="94"/>
+      <c r="E2" s="105" t="s">
         <v>64</v>
       </c>
-      <c r="F2" s="104"/>
+      <c r="F2" s="105"/>
       <c r="G2" s="4"/>
       <c r="H2" s="20"/>
       <c r="I2" s="48"/>
@@ -14743,58 +14954,58 @@
       <c r="W3" s="26"/>
     </row>
     <row r="4" spans="1:23" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="103" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" s="98" t="s">
+      <c r="A4" s="96" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="91" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="98"/>
-      <c r="D4" s="98"/>
-      <c r="E4" s="98"/>
-      <c r="F4" s="98"/>
-      <c r="G4" s="98"/>
-      <c r="H4" s="98"/>
-      <c r="I4" s="98"/>
-      <c r="J4" s="98" t="s">
+      <c r="C4" s="91"/>
+      <c r="D4" s="91"/>
+      <c r="E4" s="91"/>
+      <c r="F4" s="91"/>
+      <c r="G4" s="91"/>
+      <c r="H4" s="91"/>
+      <c r="I4" s="91"/>
+      <c r="J4" s="91" t="s">
         <v>6</v>
       </c>
-      <c r="K4" s="98" t="s">
+      <c r="K4" s="91" t="s">
         <v>11</v>
       </c>
-      <c r="L4" s="98"/>
-      <c r="M4" s="95" t="s">
+      <c r="L4" s="91"/>
+      <c r="M4" s="97" t="s">
         <v>42</v>
       </c>
-      <c r="N4" s="95" t="s">
+      <c r="N4" s="97" t="s">
         <v>10</v>
       </c>
-      <c r="O4" s="95" t="s">
+      <c r="O4" s="97" t="s">
         <v>7</v>
       </c>
-      <c r="P4" s="93" t="s">
+      <c r="P4" s="102" t="s">
         <v>14</v>
       </c>
-      <c r="Q4" s="95" t="s">
+      <c r="Q4" s="97" t="s">
         <v>39</v>
       </c>
-      <c r="R4" s="95" t="s">
+      <c r="R4" s="97" t="s">
         <v>53</v>
       </c>
-      <c r="S4" s="97" t="s">
+      <c r="S4" s="104" t="s">
         <v>54</v>
       </c>
       <c r="T4" s="26"/>
-      <c r="U4" s="98" t="s">
+      <c r="U4" s="91" t="s">
         <v>39</v>
       </c>
-      <c r="V4" s="98" t="s">
+      <c r="V4" s="91" t="s">
         <v>53</v>
       </c>
       <c r="W4" s="45"/>
     </row>
     <row r="5" spans="1:23" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="103"/>
+      <c r="A5" s="96"/>
       <c r="B5" s="66" t="s">
         <v>1</v>
       </c>
@@ -14819,23 +15030,23 @@
       <c r="I5" s="50" t="s">
         <v>15</v>
       </c>
-      <c r="J5" s="98"/>
+      <c r="J5" s="91"/>
       <c r="K5" s="66" t="s">
         <v>12</v>
       </c>
       <c r="L5" s="66" t="s">
         <v>13</v>
       </c>
-      <c r="M5" s="96"/>
-      <c r="N5" s="96"/>
-      <c r="O5" s="96"/>
-      <c r="P5" s="94"/>
-      <c r="Q5" s="96"/>
-      <c r="R5" s="96"/>
-      <c r="S5" s="97"/>
+      <c r="M5" s="98"/>
+      <c r="N5" s="98"/>
+      <c r="O5" s="98"/>
+      <c r="P5" s="103"/>
+      <c r="Q5" s="98"/>
+      <c r="R5" s="98"/>
+      <c r="S5" s="104"/>
       <c r="T5" s="26"/>
-      <c r="U5" s="98"/>
-      <c r="V5" s="98"/>
+      <c r="U5" s="91"/>
+      <c r="V5" s="91"/>
       <c r="W5" s="45"/>
     </row>
     <row r="6" spans="1:23" s="11" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -14881,7 +15092,7 @@
       </c>
       <c r="S6" s="3"/>
       <c r="T6" s="67"/>
-      <c r="U6" s="90" t="s">
+      <c r="U6" s="99" t="s">
         <v>18</v>
       </c>
       <c r="V6" s="3" t="s">
@@ -14932,7 +15143,7 @@
       </c>
       <c r="S7" s="3"/>
       <c r="T7" s="67"/>
-      <c r="U7" s="91"/>
+      <c r="U7" s="100"/>
       <c r="V7" s="3" t="s">
         <v>35</v>
       </c>
@@ -14961,7 +15172,7 @@
       <c r="R8" s="2"/>
       <c r="S8" s="3"/>
       <c r="T8" s="67"/>
-      <c r="U8" s="91"/>
+      <c r="U8" s="100"/>
       <c r="V8" s="3" t="s">
         <v>21</v>
       </c>
@@ -14990,7 +15201,7 @@
       <c r="R9" s="2"/>
       <c r="S9" s="3"/>
       <c r="T9" s="67"/>
-      <c r="U9" s="91"/>
+      <c r="U9" s="100"/>
       <c r="V9" s="3" t="s">
         <v>51</v>
       </c>
@@ -15019,7 +15230,7 @@
       <c r="R10" s="2"/>
       <c r="S10" s="3"/>
       <c r="T10" s="67"/>
-      <c r="U10" s="91"/>
+      <c r="U10" s="100"/>
       <c r="V10" s="3" t="s">
         <v>31</v>
       </c>
@@ -15048,7 +15259,7 @@
       <c r="R11" s="2"/>
       <c r="S11" s="3"/>
       <c r="T11" s="67"/>
-      <c r="U11" s="91"/>
+      <c r="U11" s="100"/>
       <c r="V11" s="3" t="s">
         <v>30</v>
       </c>
@@ -15077,7 +15288,7 @@
       <c r="R12" s="2"/>
       <c r="S12" s="3"/>
       <c r="T12" s="67"/>
-      <c r="U12" s="90" t="s">
+      <c r="U12" s="99" t="s">
         <v>19</v>
       </c>
       <c r="V12" s="3" t="s">
@@ -15108,7 +15319,7 @@
       <c r="R13" s="2"/>
       <c r="S13" s="3"/>
       <c r="T13" s="67"/>
-      <c r="U13" s="91"/>
+      <c r="U13" s="100"/>
       <c r="V13" s="3" t="s">
         <v>37</v>
       </c>
@@ -15137,7 +15348,7 @@
       <c r="R14" s="2"/>
       <c r="S14" s="3"/>
       <c r="T14" s="67"/>
-      <c r="U14" s="91"/>
+      <c r="U14" s="100"/>
       <c r="V14" s="3" t="s">
         <v>36</v>
       </c>
@@ -15166,7 +15377,7 @@
       <c r="R15" s="2"/>
       <c r="S15" s="3"/>
       <c r="T15" s="13"/>
-      <c r="U15" s="91"/>
+      <c r="U15" s="100"/>
       <c r="V15" s="3" t="s">
         <v>24</v>
       </c>
@@ -15195,7 +15406,7 @@
       <c r="R16" s="2"/>
       <c r="S16" s="3"/>
       <c r="T16" s="13"/>
-      <c r="U16" s="92"/>
+      <c r="U16" s="101"/>
       <c r="V16" s="3" t="s">
         <v>25</v>
       </c>
@@ -16911,6 +17122,13 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="U6:U11"/>
+    <mergeCell ref="U12:U16"/>
+    <mergeCell ref="P4:P5"/>
+    <mergeCell ref="Q4:Q5"/>
+    <mergeCell ref="R4:R5"/>
+    <mergeCell ref="S4:S5"/>
+    <mergeCell ref="U4:U5"/>
     <mergeCell ref="V4:V5"/>
     <mergeCell ref="A1:V1"/>
     <mergeCell ref="A2:D2"/>
@@ -16922,13 +17140,6 @@
     <mergeCell ref="M4:M5"/>
     <mergeCell ref="N4:N5"/>
     <mergeCell ref="O4:O5"/>
-    <mergeCell ref="U6:U11"/>
-    <mergeCell ref="U12:U16"/>
-    <mergeCell ref="P4:P5"/>
-    <mergeCell ref="Q4:Q5"/>
-    <mergeCell ref="R4:R5"/>
-    <mergeCell ref="S4:S5"/>
-    <mergeCell ref="U4:U5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -16972,39 +17183,39 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="99"/>
-      <c r="B1" s="99"/>
-      <c r="C1" s="99"/>
-      <c r="D1" s="99"/>
-      <c r="E1" s="99"/>
-      <c r="F1" s="99"/>
-      <c r="G1" s="99"/>
-      <c r="H1" s="99"/>
-      <c r="I1" s="99"/>
-      <c r="J1" s="99"/>
-      <c r="K1" s="99"/>
-      <c r="L1" s="99"/>
-      <c r="M1" s="99"/>
-      <c r="N1" s="99"/>
-      <c r="O1" s="99"/>
-      <c r="P1" s="99"/>
-      <c r="Q1" s="99"/>
-      <c r="R1" s="99"/>
-      <c r="S1" s="99"/>
-      <c r="T1" s="99"/>
-      <c r="U1" s="99"/>
-      <c r="V1" s="99"/>
+      <c r="A1" s="92"/>
+      <c r="B1" s="92"/>
+      <c r="C1" s="92"/>
+      <c r="D1" s="92"/>
+      <c r="E1" s="92"/>
+      <c r="F1" s="92"/>
+      <c r="G1" s="92"/>
+      <c r="H1" s="92"/>
+      <c r="I1" s="92"/>
+      <c r="J1" s="92"/>
+      <c r="K1" s="92"/>
+      <c r="L1" s="92"/>
+      <c r="M1" s="92"/>
+      <c r="N1" s="92"/>
+      <c r="O1" s="92"/>
+      <c r="P1" s="92"/>
+      <c r="Q1" s="92"/>
+      <c r="R1" s="92"/>
+      <c r="S1" s="92"/>
+      <c r="T1" s="92"/>
+      <c r="U1" s="92"/>
+      <c r="V1" s="92"/>
       <c r="W1" s="44"/>
     </row>
     <row r="2" spans="1:23" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="100" t="s">
+      <c r="A2" s="93" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="101"/>
-      <c r="C2" s="101"/>
-      <c r="D2" s="101"/>
-      <c r="E2" s="104"/>
-      <c r="F2" s="104"/>
+      <c r="B2" s="94"/>
+      <c r="C2" s="94"/>
+      <c r="D2" s="94"/>
+      <c r="E2" s="105"/>
+      <c r="F2" s="105"/>
       <c r="G2" s="4"/>
       <c r="H2" s="20"/>
       <c r="I2" s="20"/>
@@ -17049,58 +17260,58 @@
       <c r="W3" s="26"/>
     </row>
     <row r="4" spans="1:23" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="103" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" s="98" t="s">
+      <c r="A4" s="96" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="91" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="98"/>
-      <c r="D4" s="98"/>
-      <c r="E4" s="98"/>
-      <c r="F4" s="98"/>
-      <c r="G4" s="98"/>
-      <c r="H4" s="98"/>
-      <c r="I4" s="98"/>
-      <c r="J4" s="98" t="s">
+      <c r="C4" s="91"/>
+      <c r="D4" s="91"/>
+      <c r="E4" s="91"/>
+      <c r="F4" s="91"/>
+      <c r="G4" s="91"/>
+      <c r="H4" s="91"/>
+      <c r="I4" s="91"/>
+      <c r="J4" s="91" t="s">
         <v>6</v>
       </c>
-      <c r="K4" s="98" t="s">
+      <c r="K4" s="91" t="s">
         <v>11</v>
       </c>
-      <c r="L4" s="98"/>
-      <c r="M4" s="95" t="s">
+      <c r="L4" s="91"/>
+      <c r="M4" s="97" t="s">
         <v>42</v>
       </c>
-      <c r="N4" s="95" t="s">
+      <c r="N4" s="97" t="s">
         <v>10</v>
       </c>
-      <c r="O4" s="98" t="s">
+      <c r="O4" s="91" t="s">
         <v>7</v>
       </c>
-      <c r="P4" s="105" t="s">
+      <c r="P4" s="106" t="s">
         <v>14</v>
       </c>
-      <c r="Q4" s="98" t="s">
+      <c r="Q4" s="91" t="s">
         <v>39</v>
       </c>
-      <c r="R4" s="98" t="s">
+      <c r="R4" s="91" t="s">
         <v>53</v>
       </c>
-      <c r="S4" s="97" t="s">
+      <c r="S4" s="104" t="s">
         <v>54</v>
       </c>
       <c r="T4" s="26"/>
-      <c r="U4" s="98" t="s">
+      <c r="U4" s="91" t="s">
         <v>39</v>
       </c>
-      <c r="V4" s="98" t="s">
+      <c r="V4" s="91" t="s">
         <v>53</v>
       </c>
       <c r="W4" s="45"/>
     </row>
     <row r="5" spans="1:23" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="103"/>
+      <c r="A5" s="96"/>
       <c r="B5" s="41" t="s">
         <v>1</v>
       </c>
@@ -17125,23 +17336,23 @@
       <c r="I5" s="41" t="s">
         <v>15</v>
       </c>
-      <c r="J5" s="98"/>
+      <c r="J5" s="91"/>
       <c r="K5" s="41" t="s">
         <v>12</v>
       </c>
       <c r="L5" s="41" t="s">
         <v>13</v>
       </c>
-      <c r="M5" s="96"/>
-      <c r="N5" s="96"/>
-      <c r="O5" s="98"/>
-      <c r="P5" s="105"/>
-      <c r="Q5" s="98"/>
-      <c r="R5" s="98"/>
-      <c r="S5" s="97"/>
+      <c r="M5" s="98"/>
+      <c r="N5" s="98"/>
+      <c r="O5" s="91"/>
+      <c r="P5" s="106"/>
+      <c r="Q5" s="91"/>
+      <c r="R5" s="91"/>
+      <c r="S5" s="104"/>
       <c r="T5" s="26"/>
-      <c r="U5" s="98"/>
-      <c r="V5" s="98"/>
+      <c r="U5" s="91"/>
+      <c r="V5" s="91"/>
       <c r="W5" s="45"/>
     </row>
     <row r="6" spans="1:23" s="11" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -17167,7 +17378,7 @@
       <c r="R6" s="37"/>
       <c r="S6" s="3"/>
       <c r="T6" s="40"/>
-      <c r="U6" s="90" t="s">
+      <c r="U6" s="99" t="s">
         <v>18</v>
       </c>
       <c r="V6" s="3" t="s">
@@ -17198,7 +17409,7 @@
       <c r="R7" s="37"/>
       <c r="S7" s="3"/>
       <c r="T7" s="40"/>
-      <c r="U7" s="91"/>
+      <c r="U7" s="100"/>
       <c r="V7" s="3" t="s">
         <v>35</v>
       </c>
@@ -17227,7 +17438,7 @@
       <c r="R8" s="37"/>
       <c r="S8" s="3"/>
       <c r="T8" s="40"/>
-      <c r="U8" s="91"/>
+      <c r="U8" s="100"/>
       <c r="V8" s="3" t="s">
         <v>21</v>
       </c>
@@ -17256,7 +17467,7 @@
       <c r="R9" s="37"/>
       <c r="S9" s="3"/>
       <c r="T9" s="40"/>
-      <c r="U9" s="91"/>
+      <c r="U9" s="100"/>
       <c r="V9" s="3" t="s">
         <v>51</v>
       </c>
@@ -17285,7 +17496,7 @@
       <c r="R10" s="37"/>
       <c r="S10" s="3"/>
       <c r="T10" s="40"/>
-      <c r="U10" s="91"/>
+      <c r="U10" s="100"/>
       <c r="V10" s="3" t="s">
         <v>31</v>
       </c>
@@ -17314,7 +17525,7 @@
       <c r="R11" s="37"/>
       <c r="S11" s="3"/>
       <c r="T11" s="40"/>
-      <c r="U11" s="91"/>
+      <c r="U11" s="100"/>
       <c r="V11" s="3" t="s">
         <v>30</v>
       </c>
@@ -17343,7 +17554,7 @@
       <c r="R12" s="37"/>
       <c r="S12" s="3"/>
       <c r="T12" s="40"/>
-      <c r="U12" s="90" t="s">
+      <c r="U12" s="99" t="s">
         <v>19</v>
       </c>
       <c r="V12" s="3" t="s">
@@ -17374,7 +17585,7 @@
       <c r="R13" s="9"/>
       <c r="S13" s="3"/>
       <c r="T13" s="40"/>
-      <c r="U13" s="91"/>
+      <c r="U13" s="100"/>
       <c r="V13" s="3" t="s">
         <v>37</v>
       </c>
@@ -17403,7 +17614,7 @@
       <c r="R14" s="37"/>
       <c r="S14" s="3"/>
       <c r="T14" s="40"/>
-      <c r="U14" s="91"/>
+      <c r="U14" s="100"/>
       <c r="V14" s="3" t="s">
         <v>36</v>
       </c>
@@ -17432,7 +17643,7 @@
       <c r="R15" s="37"/>
       <c r="S15" s="3"/>
       <c r="T15" s="13"/>
-      <c r="U15" s="91"/>
+      <c r="U15" s="100"/>
       <c r="V15" s="3" t="s">
         <v>24</v>
       </c>
@@ -17461,7 +17672,7 @@
       <c r="R16" s="37"/>
       <c r="S16" s="3"/>
       <c r="T16" s="13"/>
-      <c r="U16" s="92"/>
+      <c r="U16" s="101"/>
       <c r="V16" s="3" t="s">
         <v>25</v>
       </c>
@@ -18692,13 +18903,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="U6:U11"/>
-    <mergeCell ref="U12:U16"/>
-    <mergeCell ref="P4:P5"/>
-    <mergeCell ref="Q4:Q5"/>
-    <mergeCell ref="R4:R5"/>
-    <mergeCell ref="S4:S5"/>
-    <mergeCell ref="U4:U5"/>
     <mergeCell ref="V4:V5"/>
     <mergeCell ref="A1:V1"/>
     <mergeCell ref="A2:D2"/>
@@ -18710,6 +18914,13 @@
     <mergeCell ref="M4:M5"/>
     <mergeCell ref="N4:N5"/>
     <mergeCell ref="O4:O5"/>
+    <mergeCell ref="U6:U11"/>
+    <mergeCell ref="U12:U16"/>
+    <mergeCell ref="P4:P5"/>
+    <mergeCell ref="Q4:Q5"/>
+    <mergeCell ref="R4:R5"/>
+    <mergeCell ref="S4:S5"/>
+    <mergeCell ref="U4:U5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>